<commit_message>
All RDF Cube tests converted. Standard deviation and mean sparql queries
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="748" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,13 @@
     <sheet name="Q1" sheetId="9" r:id="rId6"/>
     <sheet name="Q2" sheetId="10" r:id="rId7"/>
     <sheet name="A-Imputed" sheetId="4" r:id="rId8"/>
-    <sheet name="C-IMPUTED" sheetId="11" r:id="rId9"/>
-    <sheet name="A-NORMALISED" sheetId="5" r:id="rId10"/>
+    <sheet name="B-Imputed" sheetId="12" r:id="rId9"/>
+    <sheet name="C-Imputed" sheetId="11" r:id="rId10"/>
+    <sheet name="D-Imputed" sheetId="13" r:id="rId11"/>
+    <sheet name="A-Normalised" sheetId="5" r:id="rId12"/>
+    <sheet name="B-Normalised" sheetId="15" r:id="rId13"/>
+    <sheet name="C-Normalised" sheetId="14" r:id="rId14"/>
+    <sheet name="D-Normalised" sheetId="16" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="267">
   <si>
     <t>Raw</t>
   </si>
@@ -822,14 +827,20 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>MEAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -877,9 +888,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -936,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -950,16 +966,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,10 +1310,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="4" t="s">
         <v>255</v>
       </c>
@@ -2584,10 +2602,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2597,49 +2615,37 @@
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>256</v>
       </c>
       <c r="C3" s="6">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D3" s="6">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="E3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="F3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="G3" s="6">
         <v>2011</v>
       </c>
-      <c r="H3" s="6">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>252</v>
       </c>
@@ -2647,8 +2653,315 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8</v>
+      </c>
+      <c r="E7" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1.1547005383792526</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>2.309401076758502</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D9" s="5">
+        <f>AVERAGE(D5:D7)</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <f>AVERAGE(E5:E7)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1.154700538379251</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="E10" s="20">
+        <f>STDEV(E5:E7)</f>
+        <v>2.309401076758502</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2666,12 +2979,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2694,7 +3007,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2719,8 +3032,263 @@
         <v>257</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="18" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -2735,7 +3303,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -2746,16 +3314,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>3</v>
       </c>
       <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>7</v>
       </c>
     </row>
@@ -2830,7 +3398,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -2845,7 +3413,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -2859,16 +3427,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>4</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>4</v>
       </c>
     </row>
@@ -2943,7 +3511,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -2958,7 +3526,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -2972,16 +3540,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>6</v>
       </c>
       <c r="D7" s="5">
         <v>8</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -3054,7 +3622,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -3069,7 +3637,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -3083,16 +3651,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>4</v>
       </c>
       <c r="D7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>8</v>
       </c>
     </row>
@@ -3115,10 +3683,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3161,7 +3729,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -3170,7 +3738,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -3178,11 +3746,29 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3204,10 +3790,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3250,7 +3836,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -3259,7 +3845,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
@@ -3267,11 +3853,29 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>2.0816659994661335</v>
       </c>
     </row>
   </sheetData>
@@ -3293,17 +3897,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
+    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3319,7 +3924,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3345,7 +3950,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -3360,13 +3965,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="15">
         <v>2</v>
       </c>
       <c r="E6" s="5">
@@ -3374,129 +3979,51 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>3</v>
       </c>
       <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="13">
+        <f>AVERAGE(E5:E7)</f>
         <v>5</v>
       </c>
-      <c r="E7" s="14">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5">
-        <v>8</v>
-      </c>
-      <c r="E7" s="18">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3514,4 +4041,151 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added normalized values and z-score sparql queries
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="748" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="554"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -13,15 +13,17 @@
     <sheet name="C-RAW" sheetId="7" r:id="rId4"/>
     <sheet name="D-Raw" sheetId="8" r:id="rId5"/>
     <sheet name="Q1" sheetId="9" r:id="rId6"/>
-    <sheet name="Q2" sheetId="10" r:id="rId7"/>
-    <sheet name="A-Imputed" sheetId="4" r:id="rId8"/>
-    <sheet name="B-Imputed" sheetId="12" r:id="rId9"/>
-    <sheet name="C-Imputed" sheetId="11" r:id="rId10"/>
-    <sheet name="D-Imputed" sheetId="13" r:id="rId11"/>
-    <sheet name="A-Normalised" sheetId="5" r:id="rId12"/>
-    <sheet name="B-Normalised" sheetId="15" r:id="rId13"/>
-    <sheet name="C-Normalised" sheetId="14" r:id="rId14"/>
-    <sheet name="D-Normalised" sheetId="16" r:id="rId15"/>
+    <sheet name="Q1-Normalized" sheetId="17" r:id="rId7"/>
+    <sheet name="Q2" sheetId="10" r:id="rId8"/>
+    <sheet name="Q2-Normalized" sheetId="18" r:id="rId9"/>
+    <sheet name="A-Imputed" sheetId="4" r:id="rId10"/>
+    <sheet name="B-Imputed" sheetId="12" r:id="rId11"/>
+    <sheet name="C-Imputed" sheetId="11" r:id="rId12"/>
+    <sheet name="D-Imputed" sheetId="13" r:id="rId13"/>
+    <sheet name="A-Normalised" sheetId="5" r:id="rId14"/>
+    <sheet name="B-Normalised" sheetId="15" r:id="rId15"/>
+    <sheet name="C-Normalised" sheetId="14" r:id="rId16"/>
+    <sheet name="D-Normalised" sheetId="16" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="270">
   <si>
     <t>Raw</t>
   </si>
@@ -834,6 +836,15 @@
   </si>
   <si>
     <t>MEAN</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Notice that the z-score formula used here is different because indicator B is Low</t>
   </si>
 </sst>
 </file>
@@ -972,12 +983,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1298,8 +1309,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C257"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A250" sqref="A250"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="A260" sqref="A260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1310,10 +1321,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
         <v>255</v>
       </c>
@@ -2508,84 +2519,102 @@
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="251" spans="1:1" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B252" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B253" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B254" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B255" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B256" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>262</v>
+      </c>
+      <c r="B257" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2605,6 +2634,301 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2747,7 +3071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -2872,7 +3196,7 @@
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <f>STDEV(E5:E7)</f>
         <v>2.309401076758502</v>
       </c>
@@ -2894,11 +3218,132 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('A-Imputed'!C$5-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('A-Imputed'!D$5-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('A-Imputed'!E$5-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('A-Imputed'!D$6-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('A-Imputed'!E$6-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('A-Imputed'!C$7-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('A-Imputed'!D$7-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('A-Imputed'!E$7-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2914,7 +3359,10 @@
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2948,19 +3396,55 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$5)/'B-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$5)/'B-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$5)/'B-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>84</v>
       </c>
+      <c r="C6" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$6)/'B-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$6)/'B-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>53</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$7)/'B-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$7)/'B-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$7)/'B-Imputed'!E$10</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2979,12 +3463,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2999,7 +3483,7 @@
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3033,43 +3517,79 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('C-Imputed'!C$5-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('C-Imputed'!D$5-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('C-Imputed'!E$5-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>84</v>
       </c>
+      <c r="C6" s="5">
+        <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('C-Imputed'!D$6-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('C-Imputed'!E$6-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>53</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('C-Imputed'!C$7-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>1.1547005383792501</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('C-Imputed'!D$7-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('C-Imputed'!E$7-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>1.1547005383792521</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>indicators</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3084,7 +3604,7 @@
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3118,104 +3638,55 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('D-Imputed'!C$5-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('D-Imputed'!D$5-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('D-Imputed'!E$5-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>84</v>
       </c>
+      <c r="C6" s="5">
+        <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('D-Imputed'!D$6-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>-1.1547005383792517</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('D-Imputed'!E$6-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>53</v>
+      <c r="C7" s="5">
+        <f>('D-Imputed'!C$7-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('D-Imputed'!D$7-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('D-Imputed'!E$7-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3759,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
@@ -3790,10 +4261,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3808,7 +4279,7 @@
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3841,7 +4312,8 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>7</v>
+        <f>('Q1'!C$5-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3849,33 +4321,17 @@
         <v>84</v>
       </c>
       <c r="C6" s="5">
-        <v>3</v>
+        <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C10" s="5">
-        <f>AVERAGE(C5:C7)</f>
-        <v>4.666666666666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="C11" s="5">
-        <f>STDEV(C5:C7)</f>
-        <v>2.0816659994661335</v>
+      <c r="C7" s="5">
+        <f>('Q1'!C$7-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3897,158 +4353,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="13">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4</v>
-      </c>
-      <c r="E7" s="13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C10" s="13">
-        <f>AVERAGE(C5:C7)</f>
-        <v>2</v>
-      </c>
-      <c r="D10" s="13">
-        <f>AVERAGE(D5:D7)</f>
-        <v>3</v>
-      </c>
-      <c r="E10" s="13">
-        <f>AVERAGE(E5:E7)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="C11" s="5">
-        <f>STDEV(C5:C7)</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <f>STDEV(D5:D7)</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <f>STDEV(E5:E7)</f>
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4058,37 +4366,31 @@
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>256</v>
       </c>
       <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>252</v>
       </c>
@@ -4096,81 +4398,139 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="5">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5">
-        <v>6</v>
-      </c>
-      <c r="E6" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
       </c>
-      <c r="D7" s="5">
-        <v>4</v>
-      </c>
-      <c r="E7" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C9" s="13">
+        <v>266</v>
+      </c>
+      <c r="C9" s="5">
         <f>AVERAGE(C5:C7)</f>
-        <v>5</v>
-      </c>
-      <c r="D9" s="13">
-        <f>AVERAGE(D5:D7)</f>
-        <v>6</v>
-      </c>
-      <c r="E9" s="13">
-        <f>AVERAGE(E5:E7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>265</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <f>STDEV(D5:D7)</f>
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
-        <f>STDEV(E5:E7)</f>
-        <v>3</v>
+        <v>2.0816659994661335</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('Q2'!C$5-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>1.1208970766356094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.80064076902543546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('Q2'!C$7-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.32025630761017432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Example xls contains a full index computation
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="554"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="554" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,12 @@
     <sheet name="B-Imputed" sheetId="12" r:id="rId11"/>
     <sheet name="C-Imputed" sheetId="11" r:id="rId12"/>
     <sheet name="D-Imputed" sheetId="13" r:id="rId13"/>
-    <sheet name="A-Normalised" sheetId="5" r:id="rId14"/>
-    <sheet name="B-Normalised" sheetId="15" r:id="rId15"/>
-    <sheet name="C-Normalised" sheetId="14" r:id="rId16"/>
-    <sheet name="D-Normalised" sheetId="16" r:id="rId17"/>
+    <sheet name="A-Normalized" sheetId="5" r:id="rId14"/>
+    <sheet name="B-Normalized" sheetId="15" r:id="rId15"/>
+    <sheet name="C-Normalized" sheetId="14" r:id="rId16"/>
+    <sheet name="D-Normalized" sheetId="16" r:id="rId17"/>
+    <sheet name="Computation" sheetId="19" r:id="rId18"/>
+    <sheet name="Rankings" sheetId="20" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="292">
   <si>
     <t>Raw</t>
   </si>
@@ -845,13 +847,83 @@
   </si>
   <si>
     <t>Notice that the z-score formula used here is different because indicator B is Low</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>DQ1</t>
+  </si>
+  <si>
+    <t>Subindex</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>ABQ2</t>
+  </si>
+  <si>
+    <t>CDQ1</t>
+  </si>
+  <si>
+    <t>Adds 8 to all scores</t>
+  </si>
+  <si>
+    <t>Multiplies weight wi * (xi + 8)...why?</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Weidgts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C </t>
+  </si>
+  <si>
+    <t>DQ2</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Subindex transformed to 1-100 scale</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Composite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -909,8 +981,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,8 +1032,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -959,11 +1056,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -988,6 +1109,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,10 +1440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:C257"/>
+  <dimension ref="A2:C268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="A260" sqref="A260"/>
+    <sheetView topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A263" sqref="A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2615,6 +2748,46 @@
       </c>
       <c r="B257" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3396,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3701,6 +3874,828 @@
       <formula1>indicators</formula1>
     </dataValidation>
   </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="5">
+        <f>'A-Normalized'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <f>'B-Normalized'!E$5</f>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>'Q2-Normalized'!C$5</f>
+        <v>1.1208970766356094</v>
+      </c>
+      <c r="E6" s="5">
+        <f>'C-Normalized'!E$5</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="F6" s="5">
+        <f>'D-Normalized'!E$5</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G6" s="5">
+        <f>'Q1-Normalized'!C$5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5">
+        <f>'A-Normalized'!E6</f>
+        <v>-1</v>
+      </c>
+      <c r="C7" s="5">
+        <f>'B-Normalized'!E6</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <f>'Q2-Normalized'!C$6</f>
+        <v>-0.80064076902543546</v>
+      </c>
+      <c r="E7" s="5">
+        <f>'C-Normalized'!E6</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="F7" s="5">
+        <f>'D-Normalized'!E6</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="G7" s="5">
+        <f>'Q1-Normalized'!C$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5">
+        <f>'A-Normalized'!E7</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <f>'B-Normalized'!E7</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <f>'Q2-Normalized'!C$7</f>
+        <v>-0.32025630761017432</v>
+      </c>
+      <c r="E8" s="5">
+        <f>'C-Normalized'!E7</f>
+        <v>1.1547005383792521</v>
+      </c>
+      <c r="F8" s="5">
+        <f>'D-Normalized'!E7</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G8" s="5">
+        <f>'Q1-Normalized'!C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="5">
+        <f>B6+8</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <f>C6+8</f>
+        <v>7</v>
+      </c>
+      <c r="D11" s="5">
+        <f>D6+8</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E11" s="5">
+        <f>E6+8</f>
+        <v>7.4226497308103738</v>
+      </c>
+      <c r="F11" s="5">
+        <f>F6+8</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G11" s="5">
+        <f>G6+8</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B7+8</f>
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <f>C7+8</f>
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <f>D7+8</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E12" s="5">
+        <f>E7+8</f>
+        <v>7.4226497308103738</v>
+      </c>
+      <c r="F12" s="5">
+        <f>F7+8</f>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G12" s="5">
+        <f>G7+8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="5">
+        <f>B8+8</f>
+        <v>9</v>
+      </c>
+      <c r="C13" s="5">
+        <f>C8+8</f>
+        <v>9</v>
+      </c>
+      <c r="D13" s="5">
+        <f>D8+8</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E13" s="5">
+        <f>E8+8</f>
+        <v>9.1547005383792524</v>
+      </c>
+      <c r="F13" s="5">
+        <f>F8+8</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G13" s="5">
+        <f>G8+8</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="21">
+        <f>IF(B$5&gt;0,B11*B$5,"")</f>
+        <v>8</v>
+      </c>
+      <c r="C16" s="21">
+        <f>IF(C$5&gt;0,C11*C$5,"")</f>
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="21">
+        <f>IF(D$5&gt;0,D11*D$5,"")</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E16" s="21">
+        <f>IF(E$5&gt;0,E11*E$5,"")</f>
+        <v>3.7113248654051869</v>
+      </c>
+      <c r="F16" s="21">
+        <f>IF(F$5&gt;0,F11*F$5,"")</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G16" s="21">
+        <f>IF(G$5&gt;0,G11*G$5,"")</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="21">
+        <f>IF(B$5&gt;0,B12*B$5,"")</f>
+        <v>7</v>
+      </c>
+      <c r="C17" s="21">
+        <f>IF(C$5&gt;0,C12*C$5,"")</f>
+        <v>4</v>
+      </c>
+      <c r="D17" s="21">
+        <f>IF(D$5&gt;0,D12*D$5,"")</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E17" s="21">
+        <f>IF(E$5&gt;0,E12*E$5,"")</f>
+        <v>3.7113248654051869</v>
+      </c>
+      <c r="F17" s="21">
+        <f>IF(F$5&gt;0,F12*F$5,"")</f>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G17" s="21">
+        <f>IF(G$5&gt;0,G12*G$5,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="21">
+        <f>IF(B$5&gt;0,B13*B$5,"")</f>
+        <v>9</v>
+      </c>
+      <c r="C18" s="21">
+        <f>IF(C$5&gt;0,C13*C$5,"")</f>
+        <v>4.5</v>
+      </c>
+      <c r="D18" s="21">
+        <f>IF(D$5&gt;0,D13*D$5,"")</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E18" s="21">
+        <f>IF(E$5&gt;0,E13*E$5,"")</f>
+        <v>4.5773502691896262</v>
+      </c>
+      <c r="F18" s="21">
+        <f>IF(F$5&gt;0,F13*F$5,"")</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G18" s="21">
+        <f>IF(G$5&gt;0,G13*G$5,"")</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="22">
+        <f>AVERAGE(B16:C16)</f>
+        <v>5.75</v>
+      </c>
+      <c r="C21" s="22">
+        <f>AVERAGE(D16)</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="D21" s="22">
+        <f>AVERAGE(E16)</f>
+        <v>3.7113248654051869</v>
+      </c>
+      <c r="E21" s="22">
+        <f>AVERAGE(F16:G16)</f>
+        <v>6.0386751345948131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="22">
+        <f>AVERAGE(B17:C17)</f>
+        <v>5.5</v>
+      </c>
+      <c r="C22" s="22">
+        <f>AVERAGE(D17)</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="D22" s="22">
+        <f>AVERAGE(E17)</f>
+        <v>3.7113248654051869</v>
+      </c>
+      <c r="E22" s="22">
+        <f>AVERAGE(F17:G17)</f>
+        <v>5.4226497308103738</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="22">
+        <f>AVERAGE(B18:C18)</f>
+        <v>6.75</v>
+      </c>
+      <c r="C23" s="22">
+        <f>AVERAGE(D18)</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="D23" s="22">
+        <f>AVERAGE(E18)</f>
+        <v>4.5773502691896262</v>
+      </c>
+      <c r="E23" s="22">
+        <f>AVERAGE(F18:G18)</f>
+        <v>6.5386751345948131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>273</v>
+      </c>
+      <c r="B26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="22">
+        <f>AVERAGE(B21:C21)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C27" s="22">
+        <f>AVERAGE(D21:E21)</f>
+        <v>4.875</v>
+      </c>
+      <c r="D27" s="24">
+        <f>SUMPRODUCT(B27:C27,B31:C31)</f>
+        <v>5.8991794153271222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="22">
+        <f>AVERAGE(B22:C22)</f>
+        <v>6.3496796154872825</v>
+      </c>
+      <c r="C28" s="22">
+        <f>AVERAGE(D22:E22)</f>
+        <v>4.5669872981077804</v>
+      </c>
+      <c r="D28" s="24">
+        <f>SUMPRODUCT(B28:C28,B31:C31)</f>
+        <v>5.2800642250595811</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="22">
+        <f>AVERAGE(B23:C23)</f>
+        <v>7.2148718461949128</v>
+      </c>
+      <c r="C29" s="22">
+        <f>AVERAGE(D23:E23)</f>
+        <v>5.5580127018922196</v>
+      </c>
+      <c r="D29" s="24">
+        <f>SUMPRODUCT(B29:C29,B31:C31)</f>
+        <v>6.2207563596132971</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31">
+        <v>0.4</v>
+      </c>
+      <c r="C31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" s="22">
+        <f>MAX(B27:B29)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C33" s="22">
+        <f>MAX(C27:C29)</f>
+        <v>5.5580127018922196</v>
+      </c>
+      <c r="D33" s="22">
+        <f>MAX(D27:D29)</f>
+        <v>6.2207563596132971</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="22">
+        <f>MIN(B27:B29)</f>
+        <v>6.3496796154872825</v>
+      </c>
+      <c r="C34" s="22">
+        <f>MIN(C27:C29)</f>
+        <v>4.5669872981077804</v>
+      </c>
+      <c r="D34" s="22">
+        <f>MIN(D27:D29)</f>
+        <v>5.2800642250595811</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>288</v>
+      </c>
+      <c r="B35" s="22">
+        <f>B33-B34</f>
+        <v>1.0857689228305221</v>
+      </c>
+      <c r="C35" s="22">
+        <f>C33-C34</f>
+        <v>0.99102540378443926</v>
+      </c>
+      <c r="D35" s="22">
+        <f>D33-D34</f>
+        <v>0.94069213455371603</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="22">
+        <f>((B27-B34)/B35)*100</f>
+        <v>100</v>
+      </c>
+      <c r="C38" s="22">
+        <f>((C27-C34)/C35)*100</f>
+        <v>31.080202456567534</v>
+      </c>
+      <c r="D38" s="22">
+        <f>((D27-D34)/D35)*100</f>
+        <v>65.814857754844766</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="22">
+        <f>((B28-B34)/B35)*100</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="22">
+        <f>((C28-C34)/C35)*100</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="22">
+        <f>((D28-D34)/D35)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="22">
+        <f>((B29-B34)/B35)*100</f>
+        <v>79.684748063348138</v>
+      </c>
+      <c r="C40" s="22">
+        <f>((C29-C34)/C35)*100</f>
+        <v>100</v>
+      </c>
+      <c r="D40" s="22">
+        <f>((D29-D34)/D35)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="23">
+        <f>RANK(Computation!B21,Computation!B$21:B$23)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="23">
+        <f>RANK(Computation!C21,Computation!C$21:C$23)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="23">
+        <f>RANK(Computation!B27,Computation!B$27:B$29)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="23">
+        <f>RANK(Computation!D21,Computation!D$21:D$23)</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="23">
+        <f>RANK(Computation!E21,Computation!E$21:E$23)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="23">
+        <f>RANK(Computation!C27,Computation!C$27:C$29)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="26">
+        <f>RANK(Computation!D27,Computation!D$27:D$29)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="23">
+        <f>RANK(Computation!B22,Computation!B$21:B$23)</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="23">
+        <f>RANK(Computation!C22,Computation!C$21:C$23)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="23">
+        <f>RANK(Computation!B28,Computation!B$27:B$29)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="23">
+        <f>RANK(Computation!D22,Computation!D$21:D$23)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="23">
+        <f>RANK(Computation!E22,Computation!E$21:E$23)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="23">
+        <f>RANK(Computation!C28,Computation!C$27:C$29)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="26">
+        <f>RANK(Computation!D28,Computation!D$27:D$29)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="23">
+        <f>RANK(Computation!B23,Computation!B$21:B$23)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="23">
+        <f>RANK(Computation!C23,Computation!C$21:C$23)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="23">
+        <f>RANK(Computation!B29,Computation!B$27:B$29)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="23">
+        <f>RANK(Computation!D23,Computation!D$21:D$23)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <f>RANK(Computation!E23,Computation!E$21:E$23)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="23">
+        <f>RANK(Computation!C29,Computation!C$27:C$29)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="26">
+        <f>RANK(Computation!D29,Computation!D$27:D$29)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added weight schemas and a simple query to calculate rankings
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" tabRatio="554" firstSheet="12" activeTab="18"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="17115" windowHeight="7875" tabRatio="554" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -888,9 +888,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Weidgts</t>
-  </si>
-  <si>
     <t xml:space="preserve">C </t>
   </si>
   <si>
@@ -913,6 +910,9 @@
   </si>
   <si>
     <t>Composite</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -1107,9 +1107,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1121,6 +1118,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1454,10 +1454,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
         <v>255</v>
       </c>
@@ -2767,12 +2767,12 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
@@ -3882,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4100,27 +4100,27 @@
         <v>209</v>
       </c>
       <c r="B11" s="5">
-        <f>B6+8</f>
+        <f t="shared" ref="B11:G13" si="0">B6+8</f>
         <v>8</v>
       </c>
       <c r="C11" s="5">
-        <f>C6+8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D11" s="5">
-        <f>D6+8</f>
+        <f t="shared" si="0"/>
         <v>9.1208970766356092</v>
       </c>
       <c r="E11" s="5">
-        <f>E6+8</f>
+        <f t="shared" si="0"/>
         <v>7.4226497308103738</v>
       </c>
       <c r="F11" s="5">
-        <f>F6+8</f>
+        <f t="shared" si="0"/>
         <v>8.5773502691896262</v>
       </c>
       <c r="G11" s="5">
-        <f>G6+8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -4129,27 +4129,27 @@
         <v>84</v>
       </c>
       <c r="B12" s="5">
-        <f>B7+8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C12" s="5">
-        <f>C7+8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D12" s="5">
-        <f>D7+8</f>
+        <f t="shared" si="0"/>
         <v>7.1993592309745642</v>
       </c>
       <c r="E12" s="5">
-        <f>E7+8</f>
+        <f t="shared" si="0"/>
         <v>7.4226497308103738</v>
       </c>
       <c r="F12" s="5">
-        <f>F7+8</f>
+        <f t="shared" si="0"/>
         <v>6.8452994616207476</v>
       </c>
       <c r="G12" s="5">
-        <f>G7+8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -4158,27 +4158,27 @@
         <v>53</v>
       </c>
       <c r="B13" s="5">
-        <f>B8+8</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C13" s="5">
-        <f>C8+8</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D13" s="5">
-        <f>D8+8</f>
+        <f t="shared" si="0"/>
         <v>7.6797436923898257</v>
       </c>
       <c r="E13" s="5">
-        <f>E8+8</f>
+        <f t="shared" si="0"/>
         <v>9.1547005383792524</v>
       </c>
       <c r="F13" s="5">
-        <f>F8+8</f>
+        <f t="shared" si="0"/>
         <v>8.5773502691896262</v>
       </c>
       <c r="G13" s="5">
-        <f>G8+8</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -4191,28 +4191,28 @@
       <c r="A16" t="s">
         <v>209</v>
       </c>
-      <c r="B16" s="21">
-        <f>IF(B$5&gt;0,B11*B$5,"")</f>
+      <c r="B16" s="20">
+        <f t="shared" ref="B16:G18" si="1">IF(B$5&gt;0,B11*B$5,"")</f>
         <v>8</v>
       </c>
-      <c r="C16" s="21">
-        <f>IF(C$5&gt;0,C11*C$5,"")</f>
+      <c r="C16" s="20">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="D16" s="21">
-        <f>IF(D$5&gt;0,D11*D$5,"")</f>
+      <c r="D16" s="20">
+        <f t="shared" si="1"/>
         <v>9.1208970766356092</v>
       </c>
-      <c r="E16" s="21">
-        <f>IF(E$5&gt;0,E11*E$5,"")</f>
+      <c r="E16" s="20">
+        <f t="shared" si="1"/>
         <v>3.7113248654051869</v>
       </c>
-      <c r="F16" s="21">
-        <f>IF(F$5&gt;0,F11*F$5,"")</f>
+      <c r="F16" s="20">
+        <f t="shared" si="1"/>
         <v>8.5773502691896262</v>
       </c>
-      <c r="G16" s="21">
-        <f>IF(G$5&gt;0,G11*G$5,"")</f>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
@@ -4220,28 +4220,28 @@
       <c r="A17" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="21">
-        <f>IF(B$5&gt;0,B12*B$5,"")</f>
+      <c r="B17" s="20">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C17" s="21">
-        <f>IF(C$5&gt;0,C12*C$5,"")</f>
+      <c r="C17" s="20">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D17" s="21">
-        <f>IF(D$5&gt;0,D12*D$5,"")</f>
+      <c r="D17" s="20">
+        <f t="shared" si="1"/>
         <v>7.1993592309745642</v>
       </c>
-      <c r="E17" s="21">
-        <f>IF(E$5&gt;0,E12*E$5,"")</f>
+      <c r="E17" s="20">
+        <f t="shared" si="1"/>
         <v>3.7113248654051869</v>
       </c>
-      <c r="F17" s="21">
-        <f>IF(F$5&gt;0,F12*F$5,"")</f>
+      <c r="F17" s="20">
+        <f t="shared" si="1"/>
         <v>6.8452994616207476</v>
       </c>
-      <c r="G17" s="21">
-        <f>IF(G$5&gt;0,G12*G$5,"")</f>
+      <c r="G17" s="20">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -4249,28 +4249,28 @@
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="21">
-        <f>IF(B$5&gt;0,B13*B$5,"")</f>
+      <c r="B18" s="20">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C18" s="21">
-        <f>IF(C$5&gt;0,C13*C$5,"")</f>
+      <c r="C18" s="20">
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="D18" s="21">
-        <f>IF(D$5&gt;0,D13*D$5,"")</f>
+      <c r="D18" s="20">
+        <f t="shared" si="1"/>
         <v>7.6797436923898257</v>
       </c>
-      <c r="E18" s="21">
-        <f>IF(E$5&gt;0,E13*E$5,"")</f>
+      <c r="E18" s="20">
+        <f t="shared" si="1"/>
         <v>4.5773502691896262</v>
       </c>
-      <c r="F18" s="21">
-        <f>IF(F$5&gt;0,F13*F$5,"")</f>
+      <c r="F18" s="20">
+        <f t="shared" si="1"/>
         <v>8.5773502691896262</v>
       </c>
-      <c r="G18" s="21">
-        <f>IF(G$5&gt;0,G13*G$5,"")</f>
+      <c r="G18" s="20">
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
     </row>
@@ -4295,19 +4295,19 @@
       <c r="A21" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="21">
         <f>AVERAGE(B16:C16)</f>
         <v>5.75</v>
       </c>
-      <c r="C21" s="22">
-        <f>AVERAGE(D16)</f>
+      <c r="C21" s="21">
+        <f t="shared" ref="C21:D23" si="2">AVERAGE(D16)</f>
         <v>9.1208970766356092</v>
       </c>
-      <c r="D21" s="22">
-        <f>AVERAGE(E16)</f>
+      <c r="D21" s="21">
+        <f t="shared" si="2"/>
         <v>3.7113248654051869</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <f>AVERAGE(F16:G16)</f>
         <v>6.0386751345948131</v>
       </c>
@@ -4316,19 +4316,19 @@
       <c r="A22" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="21">
         <f>AVERAGE(B17:C17)</f>
         <v>5.5</v>
       </c>
-      <c r="C22" s="22">
-        <f>AVERAGE(D17)</f>
+      <c r="C22" s="21">
+        <f t="shared" si="2"/>
         <v>7.1993592309745642</v>
       </c>
-      <c r="D22" s="22">
-        <f>AVERAGE(E17)</f>
+      <c r="D22" s="21">
+        <f t="shared" si="2"/>
         <v>3.7113248654051869</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <f>AVERAGE(F17:G17)</f>
         <v>5.4226497308103738</v>
       </c>
@@ -4337,19 +4337,19 @@
       <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="21">
         <f>AVERAGE(B18:C18)</f>
         <v>6.75</v>
       </c>
-      <c r="C23" s="22">
-        <f>AVERAGE(D18)</f>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
         <v>7.6797436923898257</v>
       </c>
-      <c r="D23" s="22">
-        <f>AVERAGE(E18)</f>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
         <v>4.5773502691896262</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <f>AVERAGE(F18:G18)</f>
         <v>6.5386751345948131</v>
       </c>
@@ -4365,22 +4365,22 @@
         <v>279</v>
       </c>
       <c r="D26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="21">
         <f>AVERAGE(B21:C21)</f>
         <v>7.4354485383178046</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="21">
         <f>AVERAGE(D21:E21)</f>
         <v>4.875</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <f>SUMPRODUCT(B27:C27,B31:C31)</f>
         <v>5.8991794153271222</v>
       </c>
@@ -4389,15 +4389,15 @@
       <c r="A28" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="21">
         <f>AVERAGE(B22:C22)</f>
         <v>6.3496796154872825</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="21">
         <f>AVERAGE(D22:E22)</f>
         <v>4.5669872981077804</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <f>SUMPRODUCT(B28:C28,B31:C31)</f>
         <v>5.2800642250595811</v>
       </c>
@@ -4406,22 +4406,22 @@
       <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="21">
         <f>AVERAGE(B23:C23)</f>
         <v>7.2148718461949128</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="21">
         <f>AVERAGE(D23:E23)</f>
         <v>5.5580127018922196</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <f>SUMPRODUCT(B29:C29,B31:C31)</f>
         <v>6.2207563596132971</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B31">
         <v>0.4</v>
@@ -4432,73 +4432,73 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>286</v>
-      </c>
-      <c r="B33" s="22">
+        <v>285</v>
+      </c>
+      <c r="B33" s="21">
         <f>MAX(B27:B29)</f>
         <v>7.4354485383178046</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="21">
         <f>MAX(C27:C29)</f>
         <v>5.5580127018922196</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="21">
         <f>MAX(D27:D29)</f>
         <v>6.2207563596132971</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>287</v>
-      </c>
-      <c r="B34" s="22">
+        <v>286</v>
+      </c>
+      <c r="B34" s="21">
         <f>MIN(B27:B29)</f>
         <v>6.3496796154872825</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="21">
         <f>MIN(C27:C29)</f>
         <v>4.5669872981077804</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="21">
         <f>MIN(D27:D29)</f>
         <v>5.2800642250595811</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>288</v>
-      </c>
-      <c r="B35" s="22">
+        <v>287</v>
+      </c>
+      <c r="B35" s="21">
         <f>B33-B34</f>
         <v>1.0857689228305221</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="21">
         <f>C33-C34</f>
         <v>0.99102540378443926</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="21">
         <f>D33-D34</f>
         <v>0.94069213455371603</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>209</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="21">
         <f>((B27-B34)/B35)*100</f>
         <v>100</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="21">
         <f>((C27-C34)/C35)*100</f>
         <v>31.080202456567534</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="21">
         <f>((D27-D34)/D35)*100</f>
         <v>65.814857754844766</v>
       </c>
@@ -4507,15 +4507,15 @@
       <c r="A39" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="21">
         <f>((B28-B34)/B35)*100</f>
         <v>0</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="21">
         <f>((C28-C34)/C35)*100</f>
         <v>0</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="21">
         <f>((D28-D34)/D35)*100</f>
         <v>0</v>
       </c>
@@ -4524,15 +4524,15 @@
       <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="21">
         <f>((B29-B34)/B35)*100</f>
         <v>79.684748063348138</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="21">
         <f>((C29-C34)/C35)*100</f>
         <v>100</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="21">
         <f>((D29-D34)/D35)*100</f>
         <v>100</v>
       </c>
@@ -4546,7 +4546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4569,8 +4571,8 @@
       <c r="G1" t="s">
         <v>273</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>290</v>
+      <c r="H1" s="24" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4592,39 +4594,39 @@
       <c r="G2" t="s">
         <v>279</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>291</v>
+      <c r="H2" s="24" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <f>RANK(Computation!B21,Computation!B$21:B$23)</f>
         <v>2</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <f>RANK(Computation!C21,Computation!C$21:C$23)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <f>RANK(Computation!B27,Computation!B$27:B$29)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <f>RANK(Computation!D21,Computation!D$21:D$23)</f>
         <v>2</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <f>RANK(Computation!E21,Computation!E$21:E$23)</f>
         <v>2</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="22">
         <f>RANK(Computation!C27,Computation!C$27:C$29)</f>
         <v>2</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <f>RANK(Computation!D27,Computation!D$27:D$29)</f>
         <v>2</v>
       </c>
@@ -4633,31 +4635,31 @@
       <c r="A4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <f>RANK(Computation!B22,Computation!B$21:B$23)</f>
         <v>3</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <f>RANK(Computation!C22,Computation!C$21:C$23)</f>
         <v>3</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <f>RANK(Computation!B28,Computation!B$27:B$29)</f>
         <v>3</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <f>RANK(Computation!D22,Computation!D$21:D$23)</f>
         <v>2</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <f>RANK(Computation!E22,Computation!E$21:E$23)</f>
         <v>3</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <f>RANK(Computation!C28,Computation!C$27:C$29)</f>
         <v>3</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <f>RANK(Computation!D28,Computation!D$27:D$29)</f>
         <v>3</v>
       </c>
@@ -4666,31 +4668,31 @@
       <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <f>RANK(Computation!B23,Computation!B$21:B$23)</f>
         <v>1</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <f>RANK(Computation!C23,Computation!C$21:C$23)</f>
         <v>2</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <f>RANK(Computation!B29,Computation!B$27:B$29)</f>
         <v>2</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <f>RANK(Computation!D23,Computation!D$21:D$23)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <f>RANK(Computation!E23,Computation!E$21:E$23)</f>
         <v>1</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <f>RANK(Computation!C29,Computation!C$27:C$29)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <f>RANK(Computation!D29,Computation!D$27:D$29)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added ranking and composite index
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="17115" windowHeight="7875" tabRatio="554" firstSheet="13" activeTab="17"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="17115" windowHeight="7875" tabRatio="554" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -919,9 +919,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1090,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1120,15 +1122,17 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3892,11 +3896,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4382,16 +4390,20 @@
       <c r="A27" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="28">
         <f>AVERAGE(B21:C21)</f>
         <v>7.4354485383178046</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="27">
         <f>AVERAGE(D21:E21)</f>
         <v>4.7892586438801867</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="29">
         <f>SUMPRODUCT(B27:C27,B31:C31)</f>
+        <v>5.8477346016552341</v>
+      </c>
+      <c r="E27">
+        <f>B27*0.4+C27*0.6</f>
         <v>5.8477346016552341</v>
       </c>
     </row>
@@ -4407,7 +4419,7 @@
         <f>AVERAGE(D22:E22)</f>
         <v>4.6753750336212461</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="29">
         <f>SUMPRODUCT(B28:C28,B31:C31)</f>
         <v>5.3450968663676601</v>
       </c>
@@ -4424,7 +4436,7 @@
         <f>AVERAGE(D23:E23)</f>
         <v>5.5353663224985681</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="29">
         <f>SUMPRODUCT(B29:C29,B31:C31)</f>
         <v>6.2071685319771062</v>
       </c>
@@ -4514,7 +4526,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="25" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="21">
@@ -4556,8 +4568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4581,7 +4593,7 @@
       <c r="G1" t="s">
         <v>273</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4604,7 +4616,7 @@
       <c r="G2" t="s">
         <v>279</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="23" t="s">
         <v>290</v>
       </c>
     </row>
@@ -4636,7 +4648,7 @@
         <f>RANK(Computation!C27,Computation!C$27:C$29)</f>
         <v>2</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="24">
         <f>RANK(Computation!D27,Computation!D$27:D$29)</f>
         <v>2</v>
       </c>
@@ -4669,7 +4681,7 @@
         <f>RANK(Computation!C28,Computation!C$27:C$29)</f>
         <v>3</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="24">
         <f>RANK(Computation!D28,Computation!D$27:D$29)</f>
         <v>3</v>
       </c>
@@ -4702,7 +4714,7 @@
         <f>RANK(Computation!C29,Computation!C$27:C$29)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <f>RANK(Computation!D29,Computation!D$27:D$29)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add two sheets to example.xlsx
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nacho\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="17115" windowHeight="7875" tabRatio="554" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="554" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,19 +30,21 @@
     <sheet name="C-Normalized" sheetId="14" r:id="rId16"/>
     <sheet name="D-Normalized" sheetId="16" r:id="rId17"/>
     <sheet name="Computation" sheetId="19" r:id="rId18"/>
-    <sheet name="Rankings" sheetId="20" r:id="rId19"/>
+    <sheet name="Computation1Template" sheetId="21" r:id="rId19"/>
+    <sheet name="Computation2Template" sheetId="22" r:id="rId20"/>
+    <sheet name="Rankings" sheetId="20" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="293">
   <si>
     <t>Raw</t>
   </si>
@@ -891,9 +898,6 @@
     <t xml:space="preserve">C </t>
   </si>
   <si>
-    <t>DQ2</t>
-  </si>
-  <si>
     <t>Maximum</t>
   </si>
   <si>
@@ -913,6 +917,12 @@
   </si>
   <si>
     <t>Weights</t>
+  </si>
+  <si>
+    <t>Indicators Type</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -921,9 +931,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1092,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1127,12 +1137,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,6 +1154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1451,10 +1466,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:C268"/>
+  <dimension ref="A2:C272"/>
   <sheetViews>
-    <sheetView topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A263" sqref="A263"/>
+    <sheetView topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1465,10 +1480,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="4" t="s">
         <v>255</v>
       </c>
@@ -2783,7 +2798,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
@@ -2799,6 +2814,21 @@
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2966,7 +2996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3775,9 +3805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3896,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4383,22 +4411,22 @@
         <v>279</v>
       </c>
       <c r="D26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="27">
         <f>AVERAGE(B21:C21)</f>
         <v>7.4354485383178046</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="26">
         <f>AVERAGE(D21:E21)</f>
         <v>4.7892586438801867</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <f>SUMPRODUCT(B27:C27,B31:C31)</f>
         <v>5.8477346016552341</v>
       </c>
@@ -4419,8 +4447,12 @@
         <f>AVERAGE(D22:E22)</f>
         <v>4.6753750336212461</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <f>SUMPRODUCT(B28:C28,B31:C31)</f>
+        <v>5.3450968663676601</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:E29" si="3">B28*0.4+C28*0.6</f>
         <v>5.3450968663676601</v>
       </c>
     </row>
@@ -4436,14 +4468,18 @@
         <f>AVERAGE(D23:E23)</f>
         <v>5.5353663224985681</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <f>SUMPRODUCT(B29:C29,B31:C31)</f>
         <v>6.2071685319771062</v>
       </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>6.2071685319771062</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31">
         <v>0.4</v>
@@ -4454,7 +4490,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B33" s="21">
         <f>MAX(B27:B29)</f>
@@ -4471,7 +4507,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B34" s="21">
         <f>MIN(B27:B29)</f>
@@ -4488,7 +4524,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B35" s="21">
         <f>B33-B34</f>
@@ -4505,7 +4541,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -4566,161 +4602,464 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="B1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="E1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" t="s">
-        <v>273</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
         <v>278</v>
       </c>
-      <c r="E2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" t="s">
-        <v>272</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" t="s">
         <v>279</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="30">
+        <v>1</v>
+      </c>
+      <c r="C5" s="30">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="30">
+        <v>1</v>
+      </c>
+      <c r="E5" s="30">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1</v>
+      </c>
+      <c r="G5" s="30">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="29"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="22">
-        <f>RANK(Computation!B21,Computation!B$21:B$23)</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="22">
-        <f>RANK(Computation!C21,Computation!C$21:C$23)</f>
+      <c r="B6" s="5">
+        <f>'A-Normalized'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <f>'B-Normalized'!E$5</f>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>'Q2-Normalized'!C$5</f>
+        <v>1.1208970766356094</v>
+      </c>
+      <c r="E6" s="5">
+        <f>'C-Normalized'!E$5</f>
+        <v>-0.92031569366888055</v>
+      </c>
+      <c r="F6" s="5">
+        <f>'D-Normalized'!E$5</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G6" s="5">
+        <f>'Q1-Normalized'!C$5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5">
+        <f>'A-Normalized'!E6</f>
+        <v>-1</v>
+      </c>
+      <c r="C7" s="5">
+        <f>'B-Normalized'!E6</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <f>'Q2-Normalized'!C$6</f>
+        <v>-0.80064076902543546</v>
+      </c>
+      <c r="E7" s="5">
+        <f>'C-Normalized'!E6</f>
+        <v>-0.14379932713576235</v>
+      </c>
+      <c r="F7" s="5">
+        <f>'D-Normalized'!E6</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="G7" s="5">
+        <f>'Q1-Normalized'!C$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5">
+        <f>'A-Normalized'!E7</f>
         <v>1</v>
       </c>
-      <c r="D3" s="22">
-        <f>RANK(Computation!B27,Computation!B$27:B$29)</f>
+      <c r="C8" s="5">
+        <f>'B-Normalized'!E7</f>
         <v>1</v>
       </c>
-      <c r="E3" s="22">
-        <f>RANK(Computation!D21,Computation!D$21:D$23)</f>
-        <v>3</v>
-      </c>
-      <c r="F3" s="22">
-        <f>RANK(Computation!E21,Computation!E$21:E$23)</f>
-        <v>2</v>
-      </c>
-      <c r="G3" s="22">
-        <f>RANK(Computation!C27,Computation!C$27:C$29)</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="24">
-        <f>RANK(Computation!D27,Computation!D$27:D$29)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D8" s="5">
+        <f>'Q2-Normalized'!C$7</f>
+        <v>-0.32025630761017432</v>
+      </c>
+      <c r="E8" s="5">
+        <f>'C-Normalized'!E7</f>
+        <v>1.0641150208046437</v>
+      </c>
+      <c r="F8" s="5">
+        <f>'D-Normalized'!E7</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G8" s="5">
+        <f>'Q1-Normalized'!C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B6+8</f>
+        <v>8</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" ref="C12:G12" si="0">C6+8</f>
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>7.079684306331119</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="22">
-        <f>RANK(Computation!B22,Computation!B$21:B$23)</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="22">
-        <f>RANK(Computation!C22,Computation!C$21:C$23)</f>
-        <v>3</v>
-      </c>
-      <c r="D4" s="22">
-        <f>RANK(Computation!B28,Computation!B$27:B$29)</f>
-        <v>3</v>
-      </c>
-      <c r="E4" s="22">
-        <f>RANK(Computation!D22,Computation!D$21:D$23)</f>
-        <v>2</v>
-      </c>
-      <c r="F4" s="22">
-        <f>RANK(Computation!E22,Computation!E$21:E$23)</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="22">
-        <f>RANK(Computation!C28,Computation!C$27:C$29)</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="24">
-        <f>RANK(Computation!D28,Computation!D$27:D$29)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B13" s="5">
+        <f>B7+8</f>
+        <v>7</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" ref="C13:G13" si="1">C7+8</f>
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="1"/>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>7.8562006728642375</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="22">
-        <f>RANK(Computation!B23,Computation!B$21:B$23)</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="22">
-        <f>RANK(Computation!C23,Computation!C$21:C$23)</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="22">
-        <f>RANK(Computation!B29,Computation!B$27:B$29)</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="22">
-        <f>RANK(Computation!D23,Computation!D$21:D$23)</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="22">
-        <f>RANK(Computation!E23,Computation!E$21:E$23)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="22">
-        <f>RANK(Computation!C29,Computation!C$27:C$29)</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="24">
-        <f>RANK(Computation!D29,Computation!D$27:D$29)</f>
-        <v>1</v>
+      <c r="B14" s="5">
+        <f>B8+8</f>
+        <v>9</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" ref="C14:G14" si="2">C8+8</f>
+        <v>9</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="2"/>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="2"/>
+        <v>9.0641150208046444</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="2"/>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="20">
+        <f>IF(B$5&gt;0,B12*B$5,"")</f>
+        <v>8</v>
+      </c>
+      <c r="C18" s="20">
+        <f t="shared" ref="C18:G18" si="3">IF(C$5&gt;0,C12*C$5,"")</f>
+        <v>3.5</v>
+      </c>
+      <c r="D18" s="20">
+        <f t="shared" si="3"/>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="3"/>
+        <v>3.5398421531655595</v>
+      </c>
+      <c r="F18" s="20">
+        <f t="shared" si="3"/>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="20">
+        <f>IF(B$5&gt;0,B13*B$5,"")</f>
+        <v>7</v>
+      </c>
+      <c r="C19" s="20">
+        <f t="shared" ref="C19:G19" si="4">IF(C$5&gt;0,C13*C$5,"")</f>
+        <v>4</v>
+      </c>
+      <c r="D19" s="20">
+        <f t="shared" si="4"/>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="4"/>
+        <v>3.9281003364321188</v>
+      </c>
+      <c r="F19" s="20">
+        <f t="shared" si="4"/>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="20">
+        <f>IF(B$5&gt;0,B14*B$5,"")</f>
+        <v>9</v>
+      </c>
+      <c r="C20" s="20">
+        <f t="shared" ref="C20:G20" si="5">IF(C$5&gt;0,C14*C$5,"")</f>
+        <v>4.5</v>
+      </c>
+      <c r="D20" s="20">
+        <f t="shared" si="5"/>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="5"/>
+        <v>4.5320575104023222</v>
+      </c>
+      <c r="F20" s="20">
+        <f t="shared" si="5"/>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" si="5"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A9 A90:A354 A12:A14 A18:A20">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$267:$A$268</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4:O4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$261:$A$264</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:O3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$271:$A$272</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:O2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$252:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4831,6 +5170,492 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE(Computation1Template!B$18:'Computation1Template'!C$18)</f>
+        <v>5.75</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE(Computation1Template!D$18)</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="D2" s="21">
+        <f>AVERAGE(Computation1Template!E$18)</f>
+        <v>3.5398421531655595</v>
+      </c>
+      <c r="E2" s="21">
+        <f>AVERAGE(Computation1Template!F$18:'Computation1Template'!G$18)</f>
+        <v>6.0386751345948131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="21">
+        <f>AVERAGE(Computation1Template!B$19:'Computation1Template'!C$19)</f>
+        <v>5.5</v>
+      </c>
+      <c r="C3" s="21">
+        <f>AVERAGE(Computation1Template!D$19)</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="D3" s="21">
+        <f>AVERAGE(Computation1Template!E$19)</f>
+        <v>3.9281003364321188</v>
+      </c>
+      <c r="E3" s="21">
+        <f>AVERAGE(Computation1Template!F$19:'Computation1Template'!G$19)</f>
+        <v>5.4226497308103738</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="21">
+        <f>AVERAGE(Computation1Template!B$20:'Computation1Template'!C$20)</f>
+        <v>6.75</v>
+      </c>
+      <c r="C4" s="21">
+        <f>AVERAGE(Computation1Template!D$20)</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="D4" s="21">
+        <f>AVERAGE(Computation1Template!E$20)</f>
+        <v>4.5320575104023222</v>
+      </c>
+      <c r="E4" s="21">
+        <f>AVERAGE(Computation1Template!F$20:'Computation1Template'!G$20)</f>
+        <v>6.5386751345948131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="21">
+        <f>AVERAGE(B2:C2)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C8" s="21">
+        <f>AVERAGE(D2:E2)</f>
+        <v>4.7892586438801867</v>
+      </c>
+      <c r="E8">
+        <f>SUMPRODUCT(B8:C8,B13:C13)</f>
+        <v>5.8477346016552341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="21">
+        <f t="shared" ref="B9:B10" si="0">AVERAGE(B3:C3)</f>
+        <v>6.3496796154872825</v>
+      </c>
+      <c r="C9" s="21">
+        <f t="shared" ref="C9:C10" si="1">AVERAGE(D3:E3)</f>
+        <v>4.6753750336212461</v>
+      </c>
+      <c r="E9">
+        <f>SUMPRODUCT(B9:C9,B13:C13)</f>
+        <v>5.3450968663676601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="21">
+        <f t="shared" si="0"/>
+        <v>7.2148718461949128</v>
+      </c>
+      <c r="C10" s="21">
+        <f t="shared" si="1"/>
+        <v>5.5353663224985681</v>
+      </c>
+      <c r="E10">
+        <f>SUMPRODUCT(B10:C10,B13:C13)</f>
+        <v>6.2071685319771062</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13">
+        <v>0.4</v>
+      </c>
+      <c r="C13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="21">
+        <f>MAX(B8:B10)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C15" s="21">
+        <f>MAX(C8:C10)</f>
+        <v>5.5353663224985681</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21">
+        <f t="shared" ref="E15" si="2">MAX(E8:E10)</f>
+        <v>6.2071685319771062</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="21">
+        <f>MIN(B8:B10)</f>
+        <v>6.3496796154872825</v>
+      </c>
+      <c r="C16" s="21">
+        <f>MIN(C8:C10)</f>
+        <v>4.6753750336212461</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21">
+        <f t="shared" ref="E16" si="3">MIN(E8:E10)</f>
+        <v>5.3450968663676601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="21">
+        <f>B15-B16</f>
+        <v>1.0857689228305221</v>
+      </c>
+      <c r="C17" s="21">
+        <f>C15-C16</f>
+        <v>0.85999128887732201</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21">
+        <f t="shared" ref="E17" si="4">E15-E16</f>
+        <v>0.86207166560944604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21">
+        <f>((B8-B16)/B17)*100</f>
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <f>((C8-C16)/C17)*100</f>
+        <v>13.24241439789586</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="5">((E8-E16)/E17)*100</f>
+        <v>58.305794673373427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22">
+        <f>((B9-B16)/B17)*100</f>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22" si="6">((C9-C16)/C17)*100</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>((E9-E16)/E17)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <f>((B10-B16)/B17)*100</f>
+        <v>79.684748063348138</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:E23" si="7">((C10-C16)/C17)*100</f>
+        <v>100</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4 A8:A10 A21:A23">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3" formula="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$261:$A$264</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$267:$A$268</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:C7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="22">
+        <f>RANK(Computation!B21,Computation!B$21:B$23)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="22">
+        <f>RANK(Computation!C21,Computation!C$21:C$23)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="22">
+        <f>RANK(Computation!B27,Computation!B$27:B$29)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <f>RANK(Computation!D21,Computation!D$21:D$23)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="22">
+        <f>RANK(Computation!E21,Computation!E$21:E$23)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="22">
+        <f>RANK(Computation!C27,Computation!C$27:C$29)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="24">
+        <f>RANK(Computation!D27,Computation!D$27:D$29)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="22">
+        <f>RANK(Computation!B22,Computation!B$21:B$23)</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="22">
+        <f>RANK(Computation!C22,Computation!C$21:C$23)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="22">
+        <f>RANK(Computation!B28,Computation!B$27:B$29)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="22">
+        <f>RANK(Computation!D22,Computation!D$21:D$23)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="22">
+        <f>RANK(Computation!E22,Computation!E$21:E$23)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="22">
+        <f>RANK(Computation!C28,Computation!C$27:C$29)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="24">
+        <f>RANK(Computation!D28,Computation!D$27:D$29)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="22">
+        <f>RANK(Computation!B23,Computation!B$21:B$23)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <f>RANK(Computation!C23,Computation!C$21:C$23)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="22">
+        <f>RANK(Computation!B29,Computation!B$27:B$29)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="22">
+        <f>RANK(Computation!D23,Computation!D$21:D$23)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <f>RANK(Computation!E23,Computation!E$21:E$23)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="22">
+        <f>RANK(Computation!C29,Computation!C$27:C$29)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="24">
+        <f>RANK(Computation!D29,Computation!D$27:D$29)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5283,7 +6108,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5306,7 +6131,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5482,7 +6307,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5505,7 +6330,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed FRA for FIN
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1088,10 +1088,10 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,8 +1421,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B267" sqref="B267"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1433,10 +1433,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
         <v>251</v>
       </c>
@@ -1476,18 +1476,18 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2846,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -2996,7 +2996,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -3143,7 +3143,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -3292,7 +3292,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -3439,7 +3439,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
@@ -3560,7 +3560,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
@@ -3684,7 +3684,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
@@ -3804,7 +3804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3871,7 +3873,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
@@ -3924,7 +3926,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3983,7 +3985,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5">
         <f>'A-Normalized'!E6</f>
@@ -4067,7 +4069,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4126,7 +4128,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5">
         <f>'Indicators-Normalized'!B3+8</f>
@@ -4210,7 +4212,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4275,7 +4277,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -4320,7 +4322,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4379,7 +4381,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="20">
         <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B3*Metadata!C252)</f>
@@ -4463,7 +4465,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4508,7 +4510,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
@@ -4576,7 +4578,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4607,7 +4609,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="21">
         <f>AVERAGE('Components-Weighted'!B3:'Components-Weighted'!C3)</f>
@@ -4683,7 +4685,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <f>'Subindex-Weighted'!B3*Metadata!B267+'Subindex-Weighted'!C3*Metadata!B268</f>
@@ -4715,7 +4717,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4767,7 +4769,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="25" t="s">
         <v>205</v>
       </c>
       <c r="B3" s="22">
@@ -4801,7 +4803,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="22">
         <f>RANK('Components-Weighted'!B3,'Components-Weighted'!B$2:B$4)</f>
@@ -4867,6 +4869,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4875,7 +4878,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4940,7 +4943,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -4988,7 +4991,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5053,7 +5056,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -5099,7 +5102,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5164,7 +5167,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -5212,7 +5215,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5265,7 +5268,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>7</v>
@@ -5319,7 +5322,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5373,7 +5376,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
@@ -5411,7 +5414,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5464,7 +5467,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <v>3</v>
@@ -5518,7 +5521,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5572,7 +5575,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>

</xml_diff>

<commit_message>
Change status Inputed to Imputed
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nacho\Web_Foundation_Index\computex\ontology\examples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,7 @@
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -50,9 +55,6 @@
     <t>The original data as found on the source</t>
   </si>
   <si>
-    <t>Inputed</t>
-  </si>
-  <si>
     <t>Data including the gaps, see also inputed method</t>
   </si>
   <si>
@@ -897,6 +899,9 @@
   </si>
   <si>
     <t>AverageGrowth</t>
+  </si>
+  <si>
+    <t>Imputed</t>
   </si>
 </sst>
 </file>
@@ -1421,8 +1426,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C272"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1434,16 +1439,16 @@
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1455,1244 +1460,1244 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B252" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -2700,10 +2705,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B253" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C253">
         <v>0.5</v>
@@ -2711,10 +2716,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B254" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C254">
         <v>0.5</v>
@@ -2722,10 +2727,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B255" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -2733,10 +2738,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B256" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C256">
         <v>0.5</v>
@@ -2744,10 +2749,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B257" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -2755,15 +2760,15 @@
     </row>
     <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -2771,7 +2776,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -2779,7 +2784,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -2787,7 +2792,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B264">
         <v>1</v>
@@ -2795,12 +2800,12 @@
     </row>
     <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B267">
         <v>0.4</v>
@@ -2808,7 +2813,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B268">
         <v>0.6</v>
@@ -2816,17 +2821,17 @@
     </row>
     <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2846,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2860,23 +2865,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -2890,15 +2895,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -2913,7 +2918,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -2928,7 +2933,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>3</v>
@@ -2942,7 +2947,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="13">
         <f>AVERAGE(C5:C7)</f>
@@ -2959,7 +2964,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -2996,7 +3001,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3008,23 +3013,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3038,15 +3043,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3061,7 +3066,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -3075,7 +3080,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
@@ -3089,7 +3094,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="13">
         <f>AVERAGE(C5:C7)</f>
@@ -3106,7 +3111,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -3143,7 +3148,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3155,23 +3160,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3185,15 +3190,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3208,7 +3213,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -3223,7 +3228,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>6</v>
@@ -3238,7 +3243,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="13">
         <f>AVERAGE(C5:C7)</f>
@@ -3255,7 +3260,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -3292,7 +3297,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3304,23 +3309,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3334,15 +3339,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3357,7 +3362,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -3371,7 +3376,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
@@ -3385,7 +3390,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="5">
         <f>AVERAGE(C5:C7)</f>
@@ -3402,7 +3407,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -3438,7 +3443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3451,23 +3456,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3481,15 +3486,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3507,7 +3512,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
@@ -3524,7 +3529,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('A-Imputed'!C$7-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
@@ -3572,26 +3577,26 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3605,15 +3610,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3631,7 +3636,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
@@ -3648,7 +3653,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('B-Imputed'!C$9-'B-Imputed'!C$7)/'B-Imputed'!C$10</f>
@@ -3696,23 +3701,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3726,15 +3731,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3752,7 +3757,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
@@ -3769,7 +3774,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('C-Imputed'!C$7-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
@@ -3817,23 +3822,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3847,15 +3852,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3873,7 +3878,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
@@ -3890,7 +3895,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('D-Imputed'!C$7-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
@@ -3933,30 +3938,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
         <v>254</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
         <v>255</v>
       </c>
-      <c r="D1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>256</v>
       </c>
-      <c r="F1" t="s">
-        <v>257</v>
-      </c>
       <c r="G1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5">
         <f>'A-Normalized'!E$5</f>
@@ -3985,7 +3990,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5">
         <f>'A-Normalized'!E6</f>
@@ -4014,7 +4019,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5">
         <f>'A-Normalized'!E7</f>
@@ -4076,30 +4081,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
         <v>254</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
         <v>255</v>
       </c>
-      <c r="D1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>256</v>
       </c>
-      <c r="F1" t="s">
-        <v>257</v>
-      </c>
       <c r="G1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5">
         <f>'Indicators-Normalized'!B2+8</f>
@@ -4128,7 +4133,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5">
         <f>'Indicators-Normalized'!B3+8</f>
@@ -4157,7 +4162,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5">
         <f>'Indicators-Normalized'!B4+8</f>
@@ -4224,15 +4229,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -4240,7 +4245,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -4254,15 +4259,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -4277,7 +4282,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -4288,7 +4293,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>3</v>
@@ -4329,30 +4334,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
         <v>254</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
         <v>255</v>
       </c>
-      <c r="D1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>256</v>
       </c>
-      <c r="F1" t="s">
-        <v>257</v>
-      </c>
       <c r="G1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="20">
         <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B2*Metadata!C252)</f>
@@ -4381,7 +4386,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="20">
         <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B3*Metadata!C252)</f>
@@ -4410,7 +4415,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="20">
         <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B4*Metadata!C252)</f>
@@ -4472,24 +4477,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" t="s">
         <v>267</v>
-      </c>
-      <c r="C1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$2:'Indicators-Weighted'!C$2)</f>
@@ -4510,7 +4515,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
@@ -4531,7 +4536,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
@@ -4585,18 +4590,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" t="s">
         <v>273</v>
-      </c>
-      <c r="C1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="21">
         <f>AVERAGE('Components-Weighted'!B2:'Components-Weighted'!C2)</f>
@@ -4609,7 +4614,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21">
         <f>AVERAGE('Components-Weighted'!B3:'Components-Weighted'!C3)</f>
@@ -4622,7 +4627,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="21">
         <f>AVERAGE('Components-Weighted'!B4:'Components-Weighted'!C4)</f>
@@ -4668,15 +4673,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
         <v>277</v>
-      </c>
-      <c r="B1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2">
         <f>'Subindex-Weighted'!B2*Metadata!B267+'Subindex-Weighted'!C2*Metadata!B268</f>
@@ -4685,7 +4690,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <f>'Subindex-Weighted'!B3*Metadata!B267+'Subindex-Weighted'!C3*Metadata!B268</f>
@@ -4694,7 +4699,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <f>'Subindex-Weighted'!B4*Metadata!B267+'Subindex-Weighted'!C4*Metadata!B268</f>
@@ -4724,53 +4729,53 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
         <v>269</v>
       </c>
-      <c r="E1" t="s">
-        <v>270</v>
-      </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" t="s">
         <v>267</v>
       </c>
-      <c r="C2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>273</v>
       </c>
-      <c r="E2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G2" t="s">
-        <v>274</v>
-      </c>
       <c r="H2" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="22">
         <f>RANK('Components-Weighted'!B2,'Components-Weighted'!B$2:B$4)</f>
@@ -4803,7 +4808,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="22">
         <f>RANK('Components-Weighted'!B3,'Components-Weighted'!B$2:B$4)</f>
@@ -4836,7 +4841,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="22">
         <f>RANK('Components-Weighted'!B4,'Components-Weighted'!B$2:B$4)</f>
@@ -4890,15 +4895,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -4906,7 +4911,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -4920,15 +4925,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -4943,7 +4948,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -4957,7 +4962,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
@@ -5003,15 +5008,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -5019,7 +5024,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -5033,15 +5038,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5056,13 +5061,13 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E6" s="5">
         <v>6</v>
@@ -5070,7 +5075,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>6</v>
@@ -5114,15 +5119,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -5130,7 +5135,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -5144,15 +5149,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5167,7 +5172,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -5181,7 +5186,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
@@ -5227,15 +5232,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -5243,7 +5248,7 @@
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -5251,15 +5256,15 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5268,7 +5273,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>7</v>
@@ -5276,7 +5281,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>8</v>
@@ -5284,7 +5289,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9" s="5">
         <f>AVERAGE(C5:C7)</f>
@@ -5293,7 +5298,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -5334,23 +5339,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -5358,15 +5363,15 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5376,7 +5381,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
@@ -5385,7 +5390,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('Q1'!C$7-'Q1'!C$9)/'Q1'!C$10</f>
@@ -5426,15 +5431,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -5442,7 +5447,7 @@
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -5450,15 +5455,15 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5467,7 +5472,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>3</v>
@@ -5475,7 +5480,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
@@ -5483,7 +5488,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9" s="5">
         <f>AVERAGE(C5:C7)</f>
@@ -5492,7 +5497,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
@@ -5533,23 +5538,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -5557,15 +5562,15 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -5575,7 +5580,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>
@@ -5584,7 +5589,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5">
         <f>('Q2'!C$7-'Q2'!C$9)/'Q2'!C$10</f>

</xml_diff>

<commit_message>
Changed the order in the normalized sheets
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nacho\Web_Foundation_Index\computex\ontology\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -18,17 +13,17 @@
     <sheet name="C-RAW" sheetId="7" r:id="rId4"/>
     <sheet name="D-Raw" sheetId="8" r:id="rId5"/>
     <sheet name="Q1" sheetId="9" r:id="rId6"/>
-    <sheet name="Q1-Normalized" sheetId="17" r:id="rId7"/>
-    <sheet name="Q2" sheetId="10" r:id="rId8"/>
-    <sheet name="Q2-Normalized" sheetId="18" r:id="rId9"/>
-    <sheet name="A-Imputed" sheetId="4" r:id="rId10"/>
-    <sheet name="B-Imputed" sheetId="12" r:id="rId11"/>
-    <sheet name="C-Imputed" sheetId="11" r:id="rId12"/>
-    <sheet name="D-Imputed" sheetId="13" r:id="rId13"/>
-    <sheet name="A-Normalized" sheetId="5" r:id="rId14"/>
-    <sheet name="B-Normalized" sheetId="15" r:id="rId15"/>
-    <sheet name="C-Normalized" sheetId="14" r:id="rId16"/>
-    <sheet name="D-Normalized" sheetId="16" r:id="rId17"/>
+    <sheet name="Q2" sheetId="10" r:id="rId7"/>
+    <sheet name="A-Imputed" sheetId="4" r:id="rId8"/>
+    <sheet name="B-Imputed" sheetId="12" r:id="rId9"/>
+    <sheet name="C-Imputed" sheetId="11" r:id="rId10"/>
+    <sheet name="D-Imputed" sheetId="13" r:id="rId11"/>
+    <sheet name="A-Normalized" sheetId="5" r:id="rId12"/>
+    <sheet name="B-Normalized" sheetId="15" r:id="rId13"/>
+    <sheet name="C-Normalized" sheetId="14" r:id="rId14"/>
+    <sheet name="D-Normalized" sheetId="16" r:id="rId15"/>
+    <sheet name="Q1-Normalized" sheetId="17" r:id="rId16"/>
+    <sheet name="Q2-Normalized" sheetId="18" r:id="rId17"/>
     <sheet name="Indicators-Normalized" sheetId="21" r:id="rId18"/>
     <sheet name="Indicators-Incremented" sheetId="24" r:id="rId19"/>
     <sheet name="Indicators-Weighted" sheetId="25" r:id="rId20"/>
@@ -42,7 +37,7 @@
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -907,11 +902,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1422,7 +1417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C272"/>
   <sheetViews>
@@ -1430,14 +1425,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="27.125" customWidth="1"/>
     <col min="2" max="2" width="32.75" customWidth="1"/>
     <col min="3" max="3" width="38.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="21.75">
       <c r="A2" s="26" t="s">
         <v>248</v>
       </c>
@@ -1446,12 +1441,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="25" t="s">
         <v>284</v>
       </c>
@@ -1467,7 +1462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1475,12 +1470,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="25" t="s">
         <v>282</v>
       </c>
@@ -1488,7 +1483,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="25" t="s">
         <v>283</v>
       </c>
@@ -1496,1192 +1491,1192 @@
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1">
       <c r="A104" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1">
       <c r="A136" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1">
       <c r="A152" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1">
       <c r="A153" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1">
       <c r="A154" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1">
       <c r="A155" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1">
       <c r="A156" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1">
       <c r="A157" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1">
       <c r="A158" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1">
       <c r="A159" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1">
       <c r="A160" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1">
       <c r="A161" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1">
       <c r="A162" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1">
       <c r="A163" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1">
       <c r="A164" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1">
       <c r="A165" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1">
       <c r="A166" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1">
       <c r="A167" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1">
       <c r="A168" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1">
       <c r="A169" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1">
       <c r="A170" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1">
       <c r="A171" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1">
       <c r="A172" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1">
       <c r="A173" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1">
       <c r="A174" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1">
       <c r="A175" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1">
       <c r="A176" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1">
       <c r="A177" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1">
       <c r="A178" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1">
       <c r="A179" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1">
       <c r="A180" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1">
       <c r="A181" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1">
       <c r="A182" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1">
       <c r="A183" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1">
       <c r="A184" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1">
       <c r="A185" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1">
       <c r="A186" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1">
       <c r="A187" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1">
       <c r="A188" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1">
       <c r="A189" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1">
       <c r="A190" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1">
       <c r="A191" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1">
       <c r="A192" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1">
       <c r="A193" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1">
       <c r="A194" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1">
       <c r="A195" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1">
       <c r="A196" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1">
       <c r="A197" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1">
       <c r="A198" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1">
       <c r="A199" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1">
       <c r="A200" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1">
       <c r="A201" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1">
       <c r="A202" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1">
       <c r="A203" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1">
       <c r="A204" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1">
       <c r="A205" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1">
       <c r="A206" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1">
       <c r="A207" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1">
       <c r="A208" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1">
       <c r="A209" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1">
       <c r="A210" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1">
       <c r="A211" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1">
       <c r="A212" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1">
       <c r="A213" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1">
       <c r="A214" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1">
       <c r="A215" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1">
       <c r="A216" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1">
       <c r="A217" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1">
       <c r="A218" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1">
       <c r="A219" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1">
       <c r="A220" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1">
       <c r="A221" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1">
       <c r="A222" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1">
       <c r="A223" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1">
       <c r="A224" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1">
       <c r="A225" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1">
       <c r="A226" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1">
       <c r="A227" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1">
       <c r="A228" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1">
       <c r="A229" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1">
       <c r="A230" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1">
       <c r="A231" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1">
       <c r="A232" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1">
       <c r="A233" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1">
       <c r="A234" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1">
       <c r="A235" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1">
       <c r="A236" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1">
       <c r="A237" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1">
       <c r="A238" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1">
       <c r="A239" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1">
       <c r="A240" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3">
       <c r="A242" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3">
       <c r="A243" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3">
       <c r="A245" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3">
       <c r="A246" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3">
       <c r="A247" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3">
       <c r="A248" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3">
       <c r="A249" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A251" s="1" t="s">
         <v>243</v>
       </c>
@@ -2692,7 +2687,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3">
       <c r="A252" t="s">
         <v>253</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3">
       <c r="A253" t="s">
         <v>254</v>
       </c>
@@ -2714,7 +2709,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3">
       <c r="A254" t="s">
         <v>255</v>
       </c>
@@ -2725,7 +2720,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3">
       <c r="A255" t="s">
         <v>256</v>
       </c>
@@ -2736,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3">
       <c r="A256" t="s">
         <v>244</v>
       </c>
@@ -2747,7 +2742,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>257</v>
       </c>
@@ -2758,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A260" s="1" t="s">
         <v>265</v>
       </c>
@@ -2766,7 +2761,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>266</v>
       </c>
@@ -2774,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>257</v>
       </c>
@@ -2782,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>275</v>
       </c>
@@ -2790,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3">
       <c r="A264" t="s">
         <v>267</v>
       </c>
@@ -2798,12 +2793,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A266" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3">
       <c r="A267" t="s">
         <v>272</v>
       </c>
@@ -2811,7 +2806,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>273</v>
       </c>
@@ -2819,17 +2814,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75">
       <c r="A270" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3">
       <c r="A271" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3">
       <c r="A272" t="s">
         <v>270</v>
       </c>
@@ -2848,30 +2843,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="5"/>
+    <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -2879,7 +2873,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -2893,7 +2887,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -2901,82 +2895,83 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" s="15">
         <f>AVERAGE(C6,E6)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5">
-        <v>4</v>
-      </c>
-      <c r="E7" s="13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E7" s="16">
+        <f>D7*AVERAGE(D7/C7)</f>
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
         <v>259</v>
       </c>
       <c r="C9" s="13">
         <f>AVERAGE(C5:C7)</f>
-        <v>2</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="D9" s="13">
         <f>AVERAGE(D5:D7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" s="13">
         <f>AVERAGE(E5:E7)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.5555555555555545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="B10" s="9" t="s">
         <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
-        <v>1</v>
+        <v>1.1547005383792526</v>
       </c>
       <c r="D10" s="5">
         <f>STDEV(D5:D7)</f>
-        <v>1</v>
+        <v>1.7320508075688772</v>
       </c>
       <c r="E10" s="5">
         <f>STDEV(E5:E7)</f>
-        <v>2</v>
+        <v>3.8634085890474927</v>
       </c>
     </row>
   </sheetData>
@@ -2997,29 +2992,29 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3027,7 +3022,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3041,7 +3036,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3049,36 +3044,36 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3086,44 +3081,44 @@
         <v>4</v>
       </c>
       <c r="D7" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="5">
         <f>AVERAGE(C5:C7)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D9" s="5">
+        <f>AVERAGE(D5:D7)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="13">
-        <f>AVERAGE(D5:D7)</f>
-        <v>6</v>
-      </c>
-      <c r="E9" s="13">
+      <c r="E9" s="5">
         <f>AVERAGE(E5:E7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="B10" s="9" t="s">
         <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
-        <v>1</v>
+        <v>1.154700538379251</v>
       </c>
       <c r="D10" s="5">
         <f>STDEV(D5:D7)</f>
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="E10" s="19">
         <f>STDEV(E5:E7)</f>
-        <v>3</v>
+        <v>2.309401076758502</v>
       </c>
     </row>
   </sheetData>
@@ -3144,37 +3139,37 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3188,7 +3183,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3196,83 +3191,513 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('A-Imputed'!C$5-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('A-Imputed'!D$5-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('A-Imputed'!E$5-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('A-Imputed'!D$6-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('A-Imputed'!E$6-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('A-Imputed'!C$7-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('A-Imputed'!D$7-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('A-Imputed'!E$7-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$5)/'B-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$5)/'B-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$5)/'B-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$6)/'B-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$6)/'B-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$7)/'B-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$7)/'B-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$7)/'B-Imputed'!E$10</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('C-Imputed'!C$5-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('C-Imputed'!D$5-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('C-Imputed'!E$5-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.92031569366888055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('C-Imputed'!D$6-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('C-Imputed'!E$6-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.14379932713576235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('C-Imputed'!C$7-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>1.1547005383792501</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('C-Imputed'!D$7-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('C-Imputed'!E$7-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>1.0641150208046437</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('D-Imputed'!C$5-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('D-Imputed'!D$5-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('D-Imputed'!E$5-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('D-Imputed'!D$6-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>-1.1547005383792517</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('D-Imputed'!E$6-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('D-Imputed'!C$7-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('D-Imputed'!D$7-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('D-Imputed'!E$7-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <f>('Q1'!C$5-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="15">
-        <f>AVERAGE(C6,E6)</f>
-        <v>5</v>
-      </c>
-      <c r="E6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="13">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5">
-        <v>8</v>
-      </c>
-      <c r="E7" s="16">
-        <f>D7*AVERAGE(D7/C7)</f>
-        <v>10.666666666666666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="13">
-        <f>AVERAGE(C5:C7)</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="D9" s="13">
-        <f>AVERAGE(D5:D7)</f>
-        <v>6</v>
-      </c>
-      <c r="E9" s="13">
-        <f>AVERAGE(E5:E7)</f>
-        <v>6.5555555555555545</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="5">
-        <f>STDEV(C5:C7)</f>
-        <v>1.1547005383792526</v>
-      </c>
-      <c r="D10" s="5">
-        <f>STDEV(D5:D7)</f>
-        <v>1.7320508075688772</v>
-      </c>
-      <c r="E10" s="5">
-        <f>STDEV(E5:E7)</f>
-        <v>3.8634085890474927</v>
+      <c r="C7" s="5">
+        <f>('Q1'!C$7-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3292,52 +3717,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3345,81 +3764,32 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <f>('Q2'!C$5-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>1.1208970766356094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.80064076902543546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="13">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>6</v>
-      </c>
-      <c r="E7" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="5">
-        <f>AVERAGE(C5:C7)</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="D9" s="5">
-        <f>AVERAGE(D5:D7)</f>
-        <v>5</v>
-      </c>
-      <c r="E9" s="5">
-        <f>AVERAGE(E5:E7)</f>
-        <v>6.666666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="5">
-        <f>STDEV(C5:C7)</f>
-        <v>1.154700538379251</v>
-      </c>
-      <c r="D10" s="5">
-        <f>STDEV(D5:D7)</f>
-        <v>1.7320508075688772</v>
-      </c>
-      <c r="E10" s="19">
-        <f>STDEV(E5:E7)</f>
-        <v>2.309401076758502</v>
+      <c r="C7" s="5">
+        <f>('Q2'!C$7-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.32025630761017432</v>
       </c>
     </row>
   </sheetData>
@@ -3439,504 +3809,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <f>('A-Imputed'!C$5-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <f>('A-Imputed'!D$5-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <f>('A-Imputed'!E$5-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5">
-        <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
-        <v>-1</v>
-      </c>
-      <c r="D6" s="5">
-        <f>('A-Imputed'!D$6-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
-        <v>-1</v>
-      </c>
-      <c r="E6" s="5">
-        <f>('A-Imputed'!E$6-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5">
-        <f>('A-Imputed'!C$7-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <f>('A-Imputed'!D$7-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <f>('A-Imputed'!E$7-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <f>('B-Imputed'!C$9-'B-Imputed'!C$5)/'B-Imputed'!C$10</f>
-        <v>-1</v>
-      </c>
-      <c r="D5" s="5">
-        <f>('B-Imputed'!D$9-'B-Imputed'!D$5)/'B-Imputed'!D$10</f>
-        <v>-1</v>
-      </c>
-      <c r="E5" s="5">
-        <f>('B-Imputed'!E$9-'B-Imputed'!E$5)/'B-Imputed'!E$10</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5">
-        <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <f>('B-Imputed'!D$9-'B-Imputed'!D$6)/'B-Imputed'!D$10</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <f>('B-Imputed'!E$9-'B-Imputed'!E$6)/'B-Imputed'!E$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5">
-        <f>('B-Imputed'!C$9-'B-Imputed'!C$7)/'B-Imputed'!C$10</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <f>('B-Imputed'!D$9-'B-Imputed'!D$7)/'B-Imputed'!D$10</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <f>('B-Imputed'!E$9-'B-Imputed'!E$7)/'B-Imputed'!E$10</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <f>('C-Imputed'!C$5-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
-        <v>-0.57735026918962551</v>
-      </c>
-      <c r="D5" s="5">
-        <f>('C-Imputed'!D$5-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
-        <v>-0.57735026918962584</v>
-      </c>
-      <c r="E5" s="5">
-        <f>('C-Imputed'!E$5-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
-        <v>-0.92031569366888055</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5">
-        <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
-        <v>-0.57735026918962551</v>
-      </c>
-      <c r="D6" s="5">
-        <f>('C-Imputed'!D$6-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
-        <v>-0.57735026918962584</v>
-      </c>
-      <c r="E6" s="5">
-        <f>('C-Imputed'!E$6-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
-        <v>-0.14379932713576235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5">
-        <f>('C-Imputed'!C$7-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
-        <v>1.1547005383792501</v>
-      </c>
-      <c r="D7" s="5">
-        <f>('C-Imputed'!D$7-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
-        <v>1.1547005383792517</v>
-      </c>
-      <c r="E7" s="5">
-        <f>('C-Imputed'!E$7-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
-        <v>1.0641150208046437</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <f>('D-Imputed'!C$5-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="D5" s="5">
-        <f>('D-Imputed'!D$5-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="E5" s="5">
-        <f>('D-Imputed'!E$5-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5">
-        <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
-        <v>-1.1547005383792521</v>
-      </c>
-      <c r="D6" s="5">
-        <f>('D-Imputed'!D$6-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
-        <v>-1.1547005383792517</v>
-      </c>
-      <c r="E6" s="5">
-        <f>('D-Imputed'!E$6-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
-        <v>-1.1547005383792521</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5">
-        <f>('D-Imputed'!C$7-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="D7" s="5">
-        <f>('D-Imputed'!D$7-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="E7" s="5">
-        <f>('D-Imputed'!E$7-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
-        <v>0.57735026918962584</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3959,7 +3842,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -3988,7 +3871,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4017,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4070,16 +3953,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4102,7 +3985,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4131,7 +4014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4160,7 +4043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4213,21 +4096,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4235,7 +4118,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4243,7 +4126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4257,7 +4140,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4265,7 +4148,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="17" t="s">
         <v>204</v>
       </c>
@@ -4280,7 +4163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="11" t="s">
         <v>78</v>
       </c>
@@ -4291,7 +4174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="11" t="s">
         <v>48</v>
       </c>
@@ -4323,16 +4206,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4355,7 +4238,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4384,7 +4267,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4413,7 +4296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4466,16 +4349,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>269</v>
       </c>
@@ -4492,7 +4375,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4513,7 +4396,7 @@
         <v>6.0386751345948131</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4534,7 +4417,7 @@
         <v>5.4226497308103738</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4579,16 +4462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>268</v>
       </c>
@@ -4599,7 +4482,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4612,7 +4495,7 @@
         <v>4.7892586438801867</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4625,7 +4508,7 @@
         <v>4.6753750336212461</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4662,16 +4545,16 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>276</v>
       </c>
@@ -4679,7 +4562,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4688,7 +4571,7 @@
         <v>5.8477346016552341</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4697,7 +4580,7 @@
         <v>5.3450968663676601</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4718,16 +4601,16 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>269</v>
       </c>
@@ -4750,7 +4633,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>266</v>
       </c>
@@ -4773,7 +4656,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="25" t="s">
         <v>204</v>
       </c>
@@ -4806,7 +4689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -4839,7 +4722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4879,21 +4762,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4901,7 +4784,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4909,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4923,7 +4806,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4931,7 +4814,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -4946,7 +4829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -4960,7 +4843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -4992,21 +4875,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5014,7 +4897,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5022,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5036,7 +4919,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5044,7 +4927,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -5059,7 +4942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -5073,7 +4956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -5103,21 +4986,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5125,7 +5008,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5133,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5147,7 +5030,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5155,7 +5038,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -5170,7 +5053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -5184,7 +5067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -5216,21 +5099,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5238,7 +5121,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5246,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5254,7 +5137,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5262,7 +5145,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -5271,7 +5154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -5279,7 +5162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -5287,7 +5170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="B9" s="9" t="s">
         <v>261</v>
       </c>
@@ -5296,7 +5179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="B10" s="9" t="s">
         <v>260</v>
       </c>
@@ -5323,37 +5206,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5361,7 +5244,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5369,32 +5252,47 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <f>('Q1'!C$5-'Q1'!C$9)/'Q1'!C$10</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5">
-        <f>('Q1'!C$7-'Q1'!C$9)/'Q1'!C$10</f>
-        <v>1</v>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>2.0816659994661335</v>
       </c>
     </row>
   </sheetData>
@@ -5415,45 +5313,52 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
+    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5461,47 +5366,82 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <f>AVERAGE(C6,E6)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="13">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="5">
+        <v>259</v>
+      </c>
+      <c r="C9" s="13">
         <f>AVERAGE(C5:C7)</f>
-        <v>4.666666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="B10" s="9" t="s">
         <v>260</v>
       </c>
       <c r="C10" s="5">
         <f>STDEV(C5:C7)</f>
-        <v>2.0816659994661335</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5522,45 +5462,51 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5568,32 +5514,81 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <f>('Q2'!C$5-'Q2'!C$9)/'Q2'!C$10</f>
-        <v>1.1208970766356094</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>
-        <v>-0.80064076902543546</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5">
-        <f>('Q2'!C$7-'Q2'!C$9)/'Q2'!C$10</f>
-        <v>-0.32025630761017432</v>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Color change of Mean and SD in example.xlsx
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -910,7 +910,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -987,6 +987,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1058,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1097,6 +1103,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3115,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3215,35 +3224,37 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="30">
         <f>AVERAGE(C5:C8)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="30">
         <f>AVERAGE(D5:D8)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="30">
         <f>AVERAGE(E5:E8)</f>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C8)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="28">
         <f>STDEV(D5:D8)</f>
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="28">
         <f>STDEV(E5:E8)</f>
         <v>2</v>
       </c>
@@ -3270,7 +3281,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3362,35 +3373,37 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="30">
         <f>AVERAGE(C5:C7)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="30">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="30">
         <f>AVERAGE(E5:E7)</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C7)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="28">
         <f>STDEV(D5:D7)</f>
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="28">
         <f>STDEV(E5:E7)</f>
         <v>3</v>
       </c>
@@ -3417,7 +3430,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3511,35 +3524,35 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="30">
         <f>AVERAGE(C5:C7)</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="30">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="30">
         <f>AVERAGE(E5:E7)</f>
         <v>6.5555555555555545</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C7)</f>
         <v>1.1547005383792526</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="28">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="28">
         <f>STDEV(E5:E7)</f>
         <v>3.8634085890474927</v>
       </c>
@@ -3565,8 +3578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3658,35 +3671,37 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="28">
         <f>AVERAGE(C5:C7)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="28">
         <f>AVERAGE(D5:D7)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="28">
         <f>AVERAGE(E5:E7)</f>
         <v>6.666666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C7)</f>
         <v>1.154700538379251</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="28">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="28">
         <f>STDEV(E5:E7)</f>
         <v>2.309401076758502</v>
       </c>
@@ -5777,7 +5792,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5853,19 +5868,21 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="28">
         <f>AVERAGE(C5:C8)</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C8)</f>
         <v>2.1602468994692869</v>
       </c>
@@ -5892,7 +5909,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5968,19 +5985,21 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="28">
         <f>AVERAGE(C5:C8)</f>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f>STDEV(C5:C8)</f>
         <v>2.1602468994692869</v>
       </c>

</xml_diff>

<commit_message>
All the index is computed now
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="24" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
     <sheet name="Indicators-Normalized" sheetId="21" r:id="rId22"/>
     <sheet name="Indicators-Adjusted" sheetId="24" r:id="rId23"/>
     <sheet name="Indicators-Weighted" sheetId="25" r:id="rId24"/>
-    <sheet name="Clusters-Weighted" sheetId="22" r:id="rId25"/>
-    <sheet name="Subindex-Weighted" sheetId="26" r:id="rId26"/>
-    <sheet name="Index-Weighted" sheetId="27" r:id="rId27"/>
+    <sheet name="Clusters-Grouped" sheetId="22" r:id="rId25"/>
+    <sheet name="Subindex-Grouped" sheetId="26" r:id="rId26"/>
+    <sheet name="Composite" sheetId="27" r:id="rId27"/>
     <sheet name="Rankings" sheetId="20" r:id="rId28"/>
   </sheets>
   <definedNames>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="285">
   <si>
     <t>Raw</t>
   </si>
@@ -1100,12 +1100,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1447,10 +1447,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="4" t="s">
         <v>250</v>
       </c>
@@ -3224,37 +3224,37 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C8)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D8)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E8)</f>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <f>STDEV(D5:D8)</f>
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <f>STDEV(E5:E8)</f>
         <v>2</v>
       </c>
@@ -3373,37 +3373,37 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C7)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E7)</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>2</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>3</v>
       </c>
@@ -3524,35 +3524,35 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C7)</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E7)</f>
         <v>6.5555555555555545</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1.1547005383792526</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>3.8634085890474927</v>
       </c>
@@ -3578,7 +3578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
@@ -3671,37 +3671,37 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C7)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <f>AVERAGE(D5:D7)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <f>AVERAGE(E5:E7)</f>
         <v>6.666666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1.154700538379251</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>2.309401076758502</v>
       </c>
@@ -4970,10 +4970,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -4995,86 +4995,65 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B2">
-        <f>Metadata!B261</f>
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>Metadata!B262</f>
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f>Metadata!B263</f>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>Metadata!B263</f>
-        <v>1</v>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
+        <v>5.75</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!D3)</f>
+        <v>9.3887301496588265</v>
+      </c>
+      <c r="D2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!E3)</f>
+        <v>3.5398421531655595</v>
+      </c>
+      <c r="E2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!G3:'Indicators-Weighted'!F3)</f>
+        <v>6.2886751345948131</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
-        <v>5.75</v>
+        <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
+        <v>5.5</v>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!D3)</f>
-        <v>9.3887301496588265</v>
+        <f>AVERAGE('Indicators-Weighted'!D4)</f>
+        <v>7.5370899501137245</v>
       </c>
       <c r="D3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!E3)</f>
-        <v>3.5398421531655595</v>
+        <f>AVERAGE('Indicators-Weighted'!E4)</f>
+        <v>3.9281003364321188</v>
       </c>
       <c r="E3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!G3:'Indicators-Weighted'!F3)</f>
-        <v>6.2886751345948131</v>
+        <f>AVERAGE('Indicators-Weighted'!G4:'Indicators-Weighted'!F4)</f>
+        <v>5.5383772432819427</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
-        <v>5.5</v>
-      </c>
-      <c r="C4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!D4)</f>
-        <v>7.5370899501137245</v>
-      </c>
-      <c r="D4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!E4)</f>
-        <v>3.9281003364321188</v>
-      </c>
-      <c r="E4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!G4:'Indicators-Weighted'!F4)</f>
-        <v>5.5383772432819427</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$5:'Indicators-Weighted'!C$5)</f>
         <v>6.75</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C4" s="21">
         <f>AVERAGE('Indicators-Weighted'!D5)</f>
         <v>8</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D4" s="21">
         <f>AVERAGE('Indicators-Weighted'!E5)</f>
         <v>4.5320575104023222</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E4" s="21">
         <f>AVERAGE('Indicators-Weighted'!G5:'Indicators-Weighted'!F5)</f>
         <v>6.5201301595379508</v>
       </c>
@@ -5082,7 +5061,7 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -5104,10 +5083,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5123,62 +5102,49 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B2">
-        <f>Metadata!B267</f>
-        <v>0.4</v>
-      </c>
-      <c r="C2">
-        <f>Metadata!B268</f>
-        <v>0.6</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Clusters-Grouped'!B2:'Clusters-Grouped'!C2)</f>
+        <v>7.5693650748294132</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE('Clusters-Grouped'!D2:'Clusters-Grouped'!E2)</f>
+        <v>4.9142586438801867</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B3:'Clusters-Weighted'!C3)</f>
-        <v>7.5693650748294132</v>
+        <f>AVERAGE('Clusters-Grouped'!B3:'Clusters-Grouped'!C3)</f>
+        <v>6.5185449750568623</v>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D3:'Clusters-Weighted'!E3)</f>
-        <v>4.9142586438801867</v>
+        <f>AVERAGE('Clusters-Grouped'!D3:'Clusters-Grouped'!E3)</f>
+        <v>4.7332387898570305</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B4" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B4:'Clusters-Weighted'!C4)</f>
-        <v>6.5185449750568623</v>
+        <f>AVERAGE('Clusters-Grouped'!B4:'Clusters-Grouped'!C4)</f>
+        <v>7.375</v>
       </c>
       <c r="C4" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D4:'Clusters-Weighted'!E4)</f>
-        <v>4.7332387898570305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B5:'Clusters-Weighted'!C5)</f>
-        <v>7.375</v>
-      </c>
-      <c r="C5" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D5:'Clusters-Weighted'!E5)</f>
+        <f>AVERAGE('Clusters-Grouped'!D4:'Clusters-Grouped'!E4)</f>
         <v>5.526093834970137</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -5203,7 +5169,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5221,7 +5187,7 @@
         <v>204</v>
       </c>
       <c r="B2">
-        <f>'Subindex-Weighted'!B3*Metadata!B267+'Subindex-Weighted'!C3*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B2*Metadata!B267+'Subindex-Grouped'!C2*Metadata!B268</f>
         <v>5.976301216259877</v>
       </c>
     </row>
@@ -5230,7 +5196,7 @@
         <v>78</v>
       </c>
       <c r="B3">
-        <f>'Subindex-Weighted'!B4*Metadata!B267+'Subindex-Weighted'!C4*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B3*Metadata!B267+'Subindex-Grouped'!C3*Metadata!B268</f>
         <v>5.4473612639369637</v>
       </c>
     </row>
@@ -5239,7 +5205,7 @@
         <v>48</v>
       </c>
       <c r="B4">
-        <f>'Subindex-Weighted'!B5*Metadata!B267+'Subindex-Weighted'!C5*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B4*Metadata!B267+'Subindex-Grouped'!C4*Metadata!B268</f>
         <v>6.2656563009820818</v>
       </c>
     </row>
@@ -5258,8 +5224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5315,31 +5281,31 @@
         <v>204</v>
       </c>
       <c r="B3" s="22">
-        <f>RANK('Clusters-Weighted'!B3,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B2,'Clusters-Grouped'!B$2:B$4)</f>
         <v>2</v>
       </c>
       <c r="C3" s="22">
-        <f>RANK('Clusters-Weighted'!C3,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C2,'Clusters-Grouped'!C$2:C$4)</f>
         <v>1</v>
       </c>
       <c r="D3" s="22">
-        <f>RANK('Subindex-Weighted'!B3,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B2,'Subindex-Grouped'!B$2:B$4)</f>
         <v>1</v>
       </c>
       <c r="E3" s="22">
-        <f>RANK('Clusters-Weighted'!D3,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D2,'Clusters-Grouped'!D$2:D$4)</f>
         <v>3</v>
       </c>
       <c r="F3" s="22">
-        <f>RANK('Clusters-Weighted'!E3,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E2,'Clusters-Grouped'!E$2:E$4)</f>
         <v>2</v>
       </c>
       <c r="G3" s="22">
-        <f>RANK('Subindex-Weighted'!C3,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C2,'Subindex-Grouped'!C$2:C$4)</f>
         <v>2</v>
       </c>
       <c r="H3" s="24">
-        <f>RANK('Index-Weighted'!B2,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B2,Composite!B$2:B$4)</f>
         <v>2</v>
       </c>
     </row>
@@ -5348,31 +5314,31 @@
         <v>78</v>
       </c>
       <c r="B4" s="22">
-        <f>RANK('Clusters-Weighted'!B4,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B3,'Clusters-Grouped'!B$2:B$4)</f>
         <v>3</v>
       </c>
       <c r="C4" s="22">
-        <f>RANK('Clusters-Weighted'!C4,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C3,'Clusters-Grouped'!C$2:C$4)</f>
         <v>3</v>
       </c>
       <c r="D4" s="22">
-        <f>RANK('Subindex-Weighted'!B4,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B3,'Subindex-Grouped'!B$2:B$4)</f>
         <v>3</v>
       </c>
       <c r="E4" s="22">
-        <f>RANK('Clusters-Weighted'!D4,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D3,'Clusters-Grouped'!D$2:D$4)</f>
         <v>2</v>
       </c>
       <c r="F4" s="22">
-        <f>RANK('Clusters-Weighted'!E4,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E3,'Clusters-Grouped'!E$2:E$4)</f>
         <v>3</v>
       </c>
       <c r="G4" s="22">
-        <f>RANK('Subindex-Weighted'!C4,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C3,'Subindex-Grouped'!C$2:C$4)</f>
         <v>3</v>
       </c>
       <c r="H4" s="24">
-        <f>RANK('Index-Weighted'!B3,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B3,Composite!B$2:B$4)</f>
         <v>3</v>
       </c>
     </row>
@@ -5381,31 +5347,31 @@
         <v>48</v>
       </c>
       <c r="B5" s="22">
-        <f>RANK('Clusters-Weighted'!B5,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B4,'Clusters-Grouped'!B$2:B$4)</f>
         <v>1</v>
       </c>
       <c r="C5" s="22">
-        <f>RANK('Clusters-Weighted'!C5,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C4,'Clusters-Grouped'!C$2:C$4)</f>
         <v>2</v>
       </c>
       <c r="D5" s="22">
-        <f>RANK('Subindex-Weighted'!B5,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B4,'Subindex-Grouped'!B$2:B$4)</f>
         <v>2</v>
       </c>
       <c r="E5" s="22">
-        <f>RANK('Clusters-Weighted'!D5,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D4,'Clusters-Grouped'!D$2:D$4)</f>
         <v>1</v>
       </c>
       <c r="F5" s="22">
-        <f>RANK('Clusters-Weighted'!E5,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E4,'Clusters-Grouped'!E$2:E$4)</f>
         <v>1</v>
       </c>
       <c r="G5" s="22">
-        <f>RANK('Subindex-Weighted'!C5,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C4,'Subindex-Grouped'!C$2:C$4)</f>
         <v>1</v>
       </c>
       <c r="H5" s="24">
-        <f>RANK('Index-Weighted'!B4,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B4,Composite!B$2:B$4)</f>
         <v>1</v>
       </c>
     </row>
@@ -5868,21 +5834,21 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C8)</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>2.1602468994692869</v>
       </c>
@@ -5985,21 +5951,21 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C8)</f>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>2.1602468994692869</v>
       </c>

</xml_diff>

<commit_message>
Raw copy of files from branch web
</commit_message>
<xml_diff>
--- a/ontology/examples/example.xlsx
+++ b/ontology/examples/example.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="26" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="23" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="A-RAW" sheetId="2" r:id="rId2"/>
     <sheet name="B-RAW" sheetId="6" r:id="rId3"/>
     <sheet name="C-RAW" sheetId="7" r:id="rId4"/>
-    <sheet name="D-Raw" sheetId="8" r:id="rId5"/>
-    <sheet name="Q1" sheetId="9" r:id="rId6"/>
-    <sheet name="Q2" sheetId="10" r:id="rId7"/>
+    <sheet name="Q1" sheetId="32" r:id="rId5"/>
+    <sheet name="Q2" sheetId="33" r:id="rId6"/>
+    <sheet name="D-Raw" sheetId="8" r:id="rId7"/>
     <sheet name="A-Imputed" sheetId="28" r:id="rId8"/>
     <sheet name="B-Imputed" sheetId="29" r:id="rId9"/>
     <sheet name="C-Imputed" sheetId="30" r:id="rId10"/>
@@ -22,8 +22,8 @@
     <sheet name="B-Sorted" sheetId="12" r:id="rId13"/>
     <sheet name="C-Sorted" sheetId="11" r:id="rId14"/>
     <sheet name="D-Sorted" sheetId="13" r:id="rId15"/>
-    <sheet name="Q1-Sorted" sheetId="32" r:id="rId16"/>
-    <sheet name="Q2-Sorted" sheetId="33" r:id="rId17"/>
+    <sheet name="Q1-Sorted" sheetId="9" r:id="rId16"/>
+    <sheet name="Q2-Sorted" sheetId="10" r:id="rId17"/>
     <sheet name="A-Normalized" sheetId="5" r:id="rId18"/>
     <sheet name="B-Normalized" sheetId="15" r:id="rId19"/>
     <sheet name="C-Normalized" sheetId="14" r:id="rId20"/>
@@ -33,9 +33,9 @@
     <sheet name="Indicators-Normalized" sheetId="21" r:id="rId24"/>
     <sheet name="Indicators-Adjusted" sheetId="24" r:id="rId25"/>
     <sheet name="Indicators-Weighted" sheetId="25" r:id="rId26"/>
-    <sheet name="Clusters-Weighted" sheetId="22" r:id="rId27"/>
-    <sheet name="Subindex-Weighted" sheetId="26" r:id="rId28"/>
-    <sheet name="Index-Weighted" sheetId="27" r:id="rId29"/>
+    <sheet name="Clusters-Grouped" sheetId="22" r:id="rId27"/>
+    <sheet name="Subindex-Grouped" sheetId="26" r:id="rId28"/>
+    <sheet name="Composite" sheetId="27" r:id="rId29"/>
     <sheet name="Rankings" sheetId="20" r:id="rId30"/>
   </sheets>
   <definedNames>
@@ -43,12 +43,12 @@
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="285">
   <si>
     <t>Raw</t>
   </si>
@@ -908,11 +908,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -989,6 +989,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1060,7 +1066,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1096,6 +1102,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1424,7 +1433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C272"/>
   <sheetViews>
@@ -1432,28 +1441,28 @@
       <selection activeCell="B267" sqref="B267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.125" customWidth="1"/>
     <col min="2" max="2" width="32.75" customWidth="1"/>
     <col min="3" max="3" width="38.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="21.75">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75">
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>284</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1477,12 +1486,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>282</v>
       </c>
@@ -1490,7 +1499,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>283</v>
       </c>
@@ -1498,1192 +1507,1192 @@
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="239" spans="1:1">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="240" spans="1:1">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>243</v>
       </c>
@@ -2694,7 +2703,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>253</v>
       </c>
@@ -2705,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>254</v>
       </c>
@@ -2716,7 +2725,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>255</v>
       </c>
@@ -2727,7 +2736,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>256</v>
       </c>
@@ -2738,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>244</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>257</v>
       </c>
@@ -2760,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>265</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>266</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>257</v>
       </c>
@@ -2784,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>275</v>
       </c>
@@ -2792,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>267</v>
       </c>
@@ -2800,12 +2809,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>272</v>
       </c>
@@ -2813,7 +2822,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>273</v>
       </c>
@@ -2821,17 +2830,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75">
+    <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>270</v>
       </c>
@@ -2850,21 +2859,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -2872,7 +2881,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -2894,7 +2903,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -2902,7 +2911,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -2917,7 +2926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -2932,7 +2941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -2947,7 +2956,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -2961,7 +2970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2984,21 +2993,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3006,7 +3015,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3036,7 +3045,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3051,7 +3060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3065,7 +3074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -3093,7 +3102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="19"/>
     </row>
   </sheetData>
@@ -3114,14 +3123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
@@ -3129,7 +3138,7 @@
     <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3137,7 +3146,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3145,7 +3154,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3197,7 +3206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3211,41 +3220,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C8)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D8)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E8)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="27">
         <f>STDEV(D5:D8)</f>
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="27">
         <f>STDEV(E5:E8)</f>
         <v>2</v>
       </c>
@@ -3268,21 +3279,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3290,7 +3301,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3298,7 +3309,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3312,7 +3323,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3320,7 +3331,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3349,7 +3360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3363,36 +3374,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C7)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E7)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>3</v>
       </c>
@@ -3415,21 +3428,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3437,7 +3450,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3445,7 +3458,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3459,7 +3472,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3467,7 +3480,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3482,7 +3495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3497,7 +3510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3512,36 +3525,36 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="29">
         <f>AVERAGE(C5:C7)</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="29">
         <f>AVERAGE(D5:D7)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="29">
         <f>AVERAGE(E5:E7)</f>
         <v>6.5555555555555545</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1.1547005383792526</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>3.8634085890474927</v>
       </c>
@@ -3564,21 +3577,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3586,7 +3599,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3594,7 +3607,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3608,7 +3621,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3616,7 +3629,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3631,7 +3644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3645,7 +3658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3659,36 +3672,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C7)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="27">
         <f>AVERAGE(D5:D7)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="27">
         <f>AVERAGE(E5:E7)</f>
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C7)</f>
         <v>1.154700538379251</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="27">
         <f>STDEV(D5:D7)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="27">
         <f>STDEV(E5:E7)</f>
         <v>2.309401076758502</v>
       </c>
@@ -3711,21 +3726,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3733,7 +3748,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3741,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3749,7 +3764,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3757,7 +3772,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3766,7 +3781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3774,7 +3789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3782,37 +3797,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C8)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
       <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3821,21 +3838,21 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3843,7 +3860,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3851,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3859,7 +3876,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3867,7 +3884,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -3876,7 +3893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -3884,7 +3901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -3892,37 +3909,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="27">
         <f>AVERAGE(C5:C8)</f>
         <v>4.666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="27">
         <f>STDEV(C5:C8)</f>
         <v>2.0816659994661335</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>indicators</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3931,21 +3950,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C5" sqref="C5:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -3953,7 +3972,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3961,7 +3980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -3975,7 +3994,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -3983,7 +4002,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>204</v>
       </c>
@@ -4001,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>78</v>
       </c>
@@ -4018,7 +4037,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>48</v>
       </c>
@@ -4052,21 +4071,21 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4077,7 +4096,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4085,7 +4104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4099,7 +4118,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4107,7 +4126,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>204</v>
       </c>
@@ -4125,7 +4144,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>78</v>
       </c>
@@ -4142,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>48</v>
       </c>
@@ -4176,21 +4195,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4198,7 +4217,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4206,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4220,7 +4239,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4228,7 +4247,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>204</v>
       </c>
@@ -4243,7 +4262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>78</v>
       </c>
@@ -4254,7 +4273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>48</v>
       </c>
@@ -4268,7 +4287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>17</v>
       </c>
@@ -4298,21 +4317,21 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4320,7 +4339,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4328,7 +4347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4342,7 +4361,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4350,7 +4369,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>204</v>
       </c>
@@ -4368,7 +4387,7 @@
         <v>-0.92031569366888055</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>78</v>
       </c>
@@ -4385,7 +4404,7 @@
         <v>-0.14379932713576235</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>48</v>
       </c>
@@ -4419,21 +4438,21 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4441,7 +4460,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4449,7 +4468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4463,7 +4482,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4471,7 +4490,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>204</v>
       </c>
@@ -4489,7 +4508,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>78</v>
       </c>
@@ -4506,7 +4525,7 @@
         <v>-1.1547005383792521</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>48</v>
       </c>
@@ -4540,21 +4559,21 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4562,7 +4581,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4570,7 +4589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4578,7 +4597,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4586,7 +4605,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -4596,7 +4615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -4605,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -4632,21 +4651,21 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4654,7 +4673,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -4662,7 +4681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -4670,7 +4689,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -4678,7 +4697,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -4688,7 +4707,7 @@
         <v>1.1208970766356094</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -4697,7 +4716,7 @@
         <v>-0.80064076902543546</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -4724,16 +4743,16 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4756,7 +4775,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4785,7 +4804,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4814,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4867,16 +4886,16 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -4899,7 +4918,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -4928,7 +4947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4957,7 +4976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -5010,16 +5029,16 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5042,7 +5061,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>274</v>
       </c>
@@ -5065,7 +5084,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -5094,7 +5113,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -5123,7 +5142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -5176,16 +5195,16 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>269</v>
       </c>
@@ -5202,86 +5221,65 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B2">
-        <f>Metadata!B261</f>
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>Metadata!B262</f>
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f>Metadata!B263</f>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>Metadata!B263</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B2" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
         <v>5.75</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C2" s="21">
         <f>AVERAGE('Indicators-Weighted'!D3)</f>
         <v>9.1208970766356092</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D2" s="21">
         <f>AVERAGE('Indicators-Weighted'!E3)</f>
         <v>3.5398421531655595</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E2" s="21">
         <f>AVERAGE('Indicators-Weighted'!G3:'Indicators-Weighted'!F3)</f>
         <v>6.0386751345948131</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B3" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
         <v>5.5</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C3" s="21">
         <f>AVERAGE('Indicators-Weighted'!D4)</f>
         <v>7.1993592309745642</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D3" s="21">
         <f>AVERAGE('Indicators-Weighted'!E4)</f>
         <v>3.9281003364321188</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E3" s="21">
         <f>AVERAGE('Indicators-Weighted'!G4:'Indicators-Weighted'!F4)</f>
         <v>5.4226497308103738</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B4" s="21">
         <f>AVERAGE('Indicators-Weighted'!B$5:'Indicators-Weighted'!C$5)</f>
         <v>6.75</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C4" s="21">
         <f>AVERAGE('Indicators-Weighted'!D5)</f>
         <v>7.6797436923898257</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D4" s="21">
         <f>AVERAGE('Indicators-Weighted'!E5)</f>
         <v>4.5320575104023222</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E4" s="21">
         <f>AVERAGE('Indicators-Weighted'!G5:'Indicators-Weighted'!F5)</f>
         <v>6.5386751345948131</v>
       </c>
@@ -5289,7 +5287,7 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -5310,16 +5308,16 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>268</v>
       </c>
@@ -5330,62 +5328,49 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B2">
-        <f>Metadata!B267</f>
-        <v>0.4</v>
-      </c>
-      <c r="C2">
-        <f>Metadata!B268</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Clusters-Grouped'!B2:'Clusters-Grouped'!C2)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE('Clusters-Grouped'!D2:'Clusters-Grouped'!E2)</f>
+        <v>4.7892586438801867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B3:'Clusters-Weighted'!C3)</f>
-        <v>7.4354485383178046</v>
+        <f>AVERAGE('Clusters-Grouped'!B3:'Clusters-Grouped'!C3)</f>
+        <v>6.3496796154872825</v>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D3:'Clusters-Weighted'!E3)</f>
-        <v>4.7892586438801867</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <f>AVERAGE('Clusters-Grouped'!D3:'Clusters-Grouped'!E3)</f>
+        <v>4.6753750336212461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B4" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B4:'Clusters-Weighted'!C4)</f>
-        <v>6.3496796154872825</v>
+        <f>AVERAGE('Clusters-Grouped'!B4:'Clusters-Grouped'!C4)</f>
+        <v>7.2148718461949128</v>
       </c>
       <c r="C4" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D4:'Clusters-Weighted'!E4)</f>
-        <v>4.6753750336212461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="21">
-        <f>AVERAGE('Clusters-Weighted'!B5:'Clusters-Weighted'!C5)</f>
-        <v>7.2148718461949128</v>
-      </c>
-      <c r="C5" s="21">
-        <f>AVERAGE('Clusters-Weighted'!D5:'Clusters-Weighted'!E5)</f>
+        <f>AVERAGE('Clusters-Grouped'!D4:'Clusters-Grouped'!E4)</f>
         <v>5.5353663224985681</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -5406,16 +5391,16 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>276</v>
       </c>
@@ -5423,30 +5408,30 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>204</v>
       </c>
       <c r="B2">
-        <f>'Subindex-Weighted'!B3*Metadata!B267+'Subindex-Weighted'!C3*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B2*Metadata!B267+'Subindex-Grouped'!C2*Metadata!B268</f>
         <v>5.8477346016552341</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
       <c r="B3">
-        <f>'Subindex-Weighted'!B4*Metadata!B267+'Subindex-Weighted'!C4*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B3*Metadata!B267+'Subindex-Grouped'!C3*Metadata!B268</f>
         <v>5.3450968663676601</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
       <c r="B4">
-        <f>'Subindex-Weighted'!B5*Metadata!B267+'Subindex-Weighted'!C5*Metadata!B268</f>
+        <f>'Subindex-Grouped'!B4*Metadata!B267+'Subindex-Grouped'!C4*Metadata!B268</f>
         <v>6.2071685319771062</v>
       </c>
     </row>
@@ -5462,21 +5447,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5484,7 +5469,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5492,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5506,7 +5491,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5514,7 +5499,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -5529,7 +5514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -5543,7 +5528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -5557,7 +5542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -5587,16 +5572,16 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>269</v>
       </c>
@@ -5619,7 +5604,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>266</v>
       </c>
@@ -5642,102 +5627,102 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>204</v>
       </c>
       <c r="B3" s="22">
-        <f>RANK('Clusters-Weighted'!B3,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B2,'Clusters-Grouped'!B$2:B$4)</f>
         <v>2</v>
       </c>
       <c r="C3" s="22">
-        <f>RANK('Clusters-Weighted'!C3,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C2,'Clusters-Grouped'!C$2:C$4)</f>
         <v>1</v>
       </c>
       <c r="D3" s="22">
-        <f>RANK('Subindex-Weighted'!B3,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B2,'Subindex-Grouped'!B$2:B$4)</f>
         <v>1</v>
       </c>
       <c r="E3" s="22">
-        <f>RANK('Clusters-Weighted'!D3,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D2,'Clusters-Grouped'!D$2:D$4)</f>
         <v>3</v>
       </c>
       <c r="F3" s="22">
-        <f>RANK('Clusters-Weighted'!E3,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E2,'Clusters-Grouped'!E$2:E$4)</f>
         <v>2</v>
       </c>
       <c r="G3" s="22">
-        <f>RANK('Subindex-Weighted'!C3,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C2,'Subindex-Grouped'!C$2:C$4)</f>
         <v>2</v>
       </c>
       <c r="H3" s="24">
-        <f>RANK('Index-Weighted'!B2,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B2,Composite!B$2:B$4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="22">
-        <f>RANK('Clusters-Weighted'!B4,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B3,'Clusters-Grouped'!B$2:B$4)</f>
         <v>3</v>
       </c>
       <c r="C4" s="22">
-        <f>RANK('Clusters-Weighted'!C4,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C3,'Clusters-Grouped'!C$2:C$4)</f>
         <v>3</v>
       </c>
       <c r="D4" s="22">
-        <f>RANK('Subindex-Weighted'!B4,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B3,'Subindex-Grouped'!B$2:B$4)</f>
         <v>3</v>
       </c>
       <c r="E4" s="22">
-        <f>RANK('Clusters-Weighted'!D4,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D3,'Clusters-Grouped'!D$2:D$4)</f>
         <v>2</v>
       </c>
       <c r="F4" s="22">
-        <f>RANK('Clusters-Weighted'!E4,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E3,'Clusters-Grouped'!E$2:E$4)</f>
         <v>3</v>
       </c>
       <c r="G4" s="22">
-        <f>RANK('Subindex-Weighted'!C4,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C3,'Subindex-Grouped'!C$2:C$4)</f>
         <v>3</v>
       </c>
       <c r="H4" s="24">
-        <f>RANK('Index-Weighted'!B3,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B3,Composite!B$2:B$4)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="22">
-        <f>RANK('Clusters-Weighted'!B5,'Clusters-Weighted'!B$3:B$5)</f>
+        <f>RANK('Clusters-Grouped'!B4,'Clusters-Grouped'!B$2:B$4)</f>
         <v>1</v>
       </c>
       <c r="C5" s="22">
-        <f>RANK('Clusters-Weighted'!C5,'Clusters-Weighted'!C$3:C$5)</f>
+        <f>RANK('Clusters-Grouped'!C4,'Clusters-Grouped'!C$2:C$4)</f>
         <v>2</v>
       </c>
       <c r="D5" s="22">
-        <f>RANK('Subindex-Weighted'!B5,'Subindex-Weighted'!B$3:B$5)</f>
+        <f>RANK('Subindex-Grouped'!B4,'Subindex-Grouped'!B$2:B$4)</f>
         <v>2</v>
       </c>
       <c r="E5" s="22">
-        <f>RANK('Clusters-Weighted'!D5,'Clusters-Weighted'!D$3:D$5)</f>
+        <f>RANK('Clusters-Grouped'!D4,'Clusters-Grouped'!D$2:D$4)</f>
         <v>1</v>
       </c>
       <c r="F5" s="22">
-        <f>RANK('Clusters-Weighted'!E5,'Clusters-Weighted'!E$3:E$5)</f>
+        <f>RANK('Clusters-Grouped'!E4,'Clusters-Grouped'!E$2:E$4)</f>
         <v>1</v>
       </c>
       <c r="G5" s="22">
-        <f>RANK('Subindex-Weighted'!C5,'Subindex-Weighted'!C$3:C$5)</f>
+        <f>RANK('Subindex-Grouped'!C4,'Subindex-Grouped'!C$2:C$4)</f>
         <v>1</v>
       </c>
       <c r="H5" s="24">
-        <f>RANK('Index-Weighted'!B4,'Index-Weighted'!B$2:B$4)</f>
+        <f>RANK(Composite!B4,Composite!B$2:B$4)</f>
         <v>1</v>
       </c>
     </row>
@@ -5748,21 +5733,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -5770,7 +5755,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5778,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -5792,7 +5777,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5800,7 +5785,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -5815,7 +5800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -5829,7 +5814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -5841,7 +5826,7 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -5871,29 +5856,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -5901,21 +5886,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -5923,59 +5902,48 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="13">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>6</v>
-      </c>
-      <c r="E7" s="13">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
         <v>3</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="27"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -5995,29 +5963,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -6025,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -6033,7 +6001,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -6041,56 +6009,48 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="5">
-        <f>AVERAGE(C5:C8)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="5">
-        <f>STDEV(C5:C8)</f>
-        <v>2.1602468994692869</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="27"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -6110,29 +6070,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -6140,15 +6100,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -6156,55 +6122,58 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="5">
-        <f>AVERAGE(C5:C8)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="5">
-        <f>STDEV(C5:C8)</f>
-        <v>2.1602468994692869</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6225,14 +6194,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
@@ -6240,7 +6209,7 @@
     <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -6248,7 +6217,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -6256,7 +6225,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -6270,7 +6239,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -6278,7 +6247,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -6293,7 +6262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -6308,7 +6277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -6322,7 +6291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -6336,7 +6305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -6359,21 +6328,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
@@ -6381,7 +6350,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -6389,7 +6358,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
@@ -6403,7 +6372,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>247</v>
       </c>
@@ -6411,7 +6380,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>204</v>
       </c>
@@ -6426,7 +6395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -6440,7 +6409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -6454,7 +6423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -6468,7 +6437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>

</xml_diff>